<commit_message>
SE SACO REPORTE PARA INFORME DE AVANCE, SE AÑADIO TIPO DE CAMBIO CON TOTAL
</commit_message>
<xml_diff>
--- a/reporte_avance.xlsx
+++ b/reporte_avance.xlsx
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E72"/>
+  <dimension ref="A1:E117"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -488,7 +488,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>45fd896</t>
+          <t>c95656c</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -498,12 +498,12 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2025-10-20</t>
+          <t>2025-11-18</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Merge pull request #8 from aycaRichard12/Feacture-punto_de_venta_cotizacion_facturacion</t>
+          <t>añadir anular Cotizacion en cuentas Sin Factura</t>
         </is>
       </c>
     </row>
@@ -513,7 +513,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>ff5c859</t>
+          <t>9763c03</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -523,12 +523,12 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2025-10-20</t>
+          <t>2025-11-18</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>[•] agregar marge adevelop</t>
+          <t>registrar precio sugerido que afecte a todos los almacenes, actulizar tabla compra al registrar automaticamente filtrar del almacen registrodo,visualizar la factura despues de registrar en factura , factura exportacion , factura alquiler, bug mostrar reporte pdf de compras por almacen</t>
         </is>
       </c>
     </row>
@@ -538,7 +538,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>5d0f3c8</t>
+          <t>44260ca</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -548,12 +548,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2025-10-20</t>
+          <t>2025-11-17</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>[•] Se añadio punto de venta a cotizaion y se muestra en los reportes tanto de venta y cotizacion</t>
+          <t>se normalizo useCotizacion que se trajabaron de prueba respuesta de emizor por defecto se quito se añadio el simbolo de moneda en reporte ventas hoy, se añadio eniviar por correo el comprobante o la factura de impuesto tambien al facturar una cotizacion se podra ver la factura despues, se mejoro el reporte para que un link de un pdf sea enviado por correo</t>
         </is>
       </c>
     </row>
@@ -563,7 +563,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>15d5fd2</t>
+          <t>6590116</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -573,12 +573,12 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2025-10-20</t>
+          <t>2025-11-17</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>[♦] PENDIENTE: SE AGREGO PUNTO DE VENTA A LOS REPORTES DE VENTAY SE REGISTRA EL PUNTO DE VENTA EN CADA COTIZACION Y SE ESTA VIENDO COLOCAR EL PUNTO DE VENTA EN LOS REPOSRTE Y FALTA REGISTRO DE ALMACEN</t>
+          <t>Arreglar cosigo sin producto, cotizacion facurar de normal y preferencial cambios de estado 2 facturado y no se puede facturar 2 veces</t>
         </is>
       </c>
     </row>
@@ -588,7 +588,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>da93671</t>
+          <t>b8cc5cb</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -598,12 +598,12 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-11-13</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Merge pull request #5 from aycaRichard12/Feacture-Cotizacion_Detalle_Adicional_Cotizacion</t>
+          <t>en App se quito la comparacion du usuario</t>
         </is>
       </c>
     </row>
@@ -613,7 +613,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>0b50aa7</t>
+          <t>25a40d2</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -623,12 +623,12 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-11-13</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>[•] GOOD: se añadio descripcion adicional a cotizacion preferencial o normal en carrito para especificar los servicios tambien se añadio numero factura o ducumento a cotizaion tambien se muestra en los reportes dichos cambios</t>
+          <t>Cambios Factura Exportacion add tipo cambio dinamico</t>
         </is>
       </c>
     </row>
@@ -638,7 +638,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>feb7ab7</t>
+          <t>63d4433</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -648,12 +648,12 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-11-13</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Merge pull request #3 from aycaRichard12/Feacture-Detalle_Venta_Cotizacion</t>
+          <t>cotizacion facturar cotizacion Normal , arreglo facturacion Comercializacion</t>
         </is>
       </c>
     </row>
@@ -663,7 +663,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>0225d73</t>
+          <t>c07fefa</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -673,12 +673,12 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-11-08</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>[•] Se agrego descripcion adicional en carrito fenta finalizado</t>
+          <t>comando por voz, correcciones comercial interfaz , se añadio filtro excel en almacen</t>
         </is>
       </c>
     </row>
@@ -688,7 +688,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>89d2b1b</t>
+          <t>c81402a</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -698,12 +698,12 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-11-06</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>[•] Se añadio descripcion adicional en carrito ventas debajo de descripcion del producto</t>
+          <t>Se arreglo cambio de estado merma</t>
         </is>
       </c>
     </row>
@@ -713,7 +713,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2caed0c</t>
+          <t>3004e31</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -723,12 +723,12 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-11-06</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>[◘] DEJAR DE RASTREAR .ENV EN DEVELOP</t>
+          <t>Se arreglo cambio de estado robo</t>
         </is>
       </c>
     </row>
@@ -738,7 +738,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>a70e993</t>
+          <t>2472148</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -748,12 +748,12 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-11-06</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>[♦♦] CONFIG: gitignore</t>
+          <t>[•] Añadir cambios anulacion cotizacion, pdf con sangria Anulado, fitrado tabla similar excel</t>
         </is>
       </c>
     </row>
@@ -763,7 +763,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>ac09b1b</t>
+          <t>3c3f990</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -773,12 +773,12 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-11-01</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Merge branch 'main' into develop</t>
+          <t>Se Actualizo bugs de errores de cotizacion como por ejemplo estado solo hay dos 0 y 1 que significa NORMAL y PREFERENCIAL y se añadio en la base de datos una columna condicion para ver si esta activa o anulada la cotizacion se realizo las pruebas respectivas, se separo la logica en 2 variables estado y condicion</t>
         </is>
       </c>
     </row>
@@ -788,7 +788,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>8c87406</t>
+          <t>be62e5c</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -798,12 +798,12 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-31</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Merge pull request #1 from aycaRichard12/Feacture-kardex</t>
+          <t>Merge pull request #17 from aycaRichard12/Feacture-Anulacion-Cotizacion</t>
         </is>
       </c>
     </row>
@@ -813,7 +813,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>40d7dc7</t>
+          <t>5a0ab7a</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -823,12 +823,12 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-31</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Merge branch 'develop' of https://github.com/aycaRichard12/Ms_comercial into Feacture-kardex</t>
+          <t>[•] ANULAR COTIZACION DE COMERCIAL, MOSTRAR EN PDF ESPECIFICAMENTE EL DOCUMENTO ANULADO LA SANGRIA</t>
         </is>
       </c>
     </row>
@@ -838,7 +838,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>8627407</t>
+          <t>e40fe0e</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -848,12 +848,12 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-30</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>[•] Completado editar saldos eliminar y modal desplegable de los saldos de un producto seleccionado</t>
+          <t>Merge pull request #15 from aycaRichard12/Feacture-Anulacion-Cotizacion</t>
         </is>
       </c>
     </row>
@@ -863,7 +863,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>2578a08</t>
+          <t>e5209e4</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -873,12 +873,12 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-30</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>[•] BUG: correccion bug componente venta se mostraba a inicio sesion apezar de que no tenia permisos para mostrar</t>
+          <t>[•] Añadir la opcion de que sea opcional el especificar el lote de la compra al registrar ROBOS y MERMAS</t>
         </is>
       </c>
     </row>
@@ -888,7 +888,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>92c2751</t>
+          <t>1175a19</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -898,12 +898,12 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-29</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>[♦] BUG MENU: se aumento en la funcion selectSubmenu otro else if para validar que si no tiene paginas el submenu entonces enrutar a la base del menu</t>
+          <t>Merge pull request #14 from aycaRichard12/Feacture-Correcciones</t>
         </is>
       </c>
     </row>
@@ -913,7 +913,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>af8a9eb</t>
+          <t>bdef3d7</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -923,12 +923,12 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-29</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>[•] Iyeccion mistersoft esta fallando venta</t>
+          <t>[•] botones asignar almacen alineados en fila</t>
         </is>
       </c>
     </row>
@@ -938,7 +938,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>bd7bea8</t>
+          <t>4c4c7c6</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -948,12 +948,12 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-29</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>[♦] Imcompleto cardex para mostrar detalle de saldo final</t>
+          <t>[•] Crear titulos para asignar almacen asignar punto de venta y asignar productos</t>
         </is>
       </c>
     </row>
@@ -963,7 +963,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>d331fac</t>
+          <t>5aac9fd</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -973,12 +973,12 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-29</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>[♦] PENDIENTE KARDEX: se logro obtener el precio unitario de cada compra y su respectivo movimiento los negativos son salidas y los positivos son movimientos</t>
+          <t>[•] Colocar Iconos a paginas de pedidos</t>
         </is>
       </c>
     </row>
@@ -988,7 +988,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>0a097e1</t>
+          <t>f45fc46</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -998,12 +998,12 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-29</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>[•] BUG: correccion bug componente venta se mostraba a inicio sesion apezar de que no tenia permisos para mostrar</t>
+          <t>[•] Etiquetas a botones de MOvimientos cambiar icon de carrito</t>
         </is>
       </c>
     </row>
@@ -1013,7 +1013,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>7a5032d</t>
+          <t>d87b7cf</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1023,12 +1023,12 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-29</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>[♦] IMCOMPLETO: NO SE TERMINO KARDEX</t>
+          <t>[•] Movimientos muestra de forma ordenada columna N°</t>
         </is>
       </c>
     </row>
@@ -1038,7 +1038,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>85ed0f8</t>
+          <t>d661372</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1048,12 +1048,12 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-29</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>[•] BUG: correccion bug componente venta se mostraba a inicio sesion apezar de que no tenia permisos para mostrar</t>
+          <t>[•] Finalizacion obtener token del emizor para la venta out</t>
         </is>
       </c>
     </row>
@@ -1063,7 +1063,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>1531505</t>
+          <t>3b28f38</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1073,12 +1073,12 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>2025-10-10</t>
+          <t>2025-10-28</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>[•] BUG PERMISOS DE MENUS: se quito el direcionamiento automatico to:/ solo se opto por el @click</t>
+          <t>[•] registrar venta por una ruta diferente en php out/venta metodo POST simplificar endpoint venta para la pagina web ya se hizo la prueba</t>
         </is>
       </c>
     </row>
@@ -1088,7 +1088,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>5b580ba</t>
+          <t>dd75382</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1098,12 +1098,12 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>2025-10-10</t>
+          <t>2025-10-28</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>[•] COMPRA: modificar los btns reposrtes en select</t>
+          <t>[•] ACTUALIZAR apis exteriores para comercial y que funciones bien</t>
         </is>
       </c>
     </row>
@@ -1113,7 +1113,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>9f1a936</t>
+          <t>1dbbaed</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1123,12 +1123,12 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>2025-10-10</t>
+          <t>2025-10-25</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>[•] FINALIZACION FACTURA NOTA CREDITO: modificacion backen nota-credito - venta, modificacion front end combinar con contingencia</t>
+          <t>Merge pull request #10 from aycaRichard12/Feacture_Kardex_saldo_inicial_x_lotes_con_saldo</t>
         </is>
       </c>
     </row>
@@ -1138,7 +1138,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>6faad43</t>
+          <t>b182dc3</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1148,12 +1148,12 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>2025-10-07</t>
+          <t>2025-10-25</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>[●] cambio tarjeta venta inicio a Resgistrar Venta</t>
+          <t>[•] Finalizacion de kardex entrara a rebicion: se modifico el metodo PROMEDIO para hacer las calculos respectivos se arreglo el bug de los reposrtes en pdf</t>
         </is>
       </c>
     </row>
@@ -1163,7 +1163,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>bad185c</t>
+          <t>07716be</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1173,12 +1173,12 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>2025-10-10</t>
+          <t>2025-10-24</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>[•] BUG PERMISOS DE MENUS: se quito el direcionamiento automatico to:/ solo se opto por el @click</t>
+          <t>Merge branch 'main' of https://github.com/aycaRichard12/Ms_comercial into Feacture_Kardex_saldo_inicial_x_lotes_con_saldo</t>
         </is>
       </c>
     </row>
@@ -1188,7 +1188,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>e285b72</t>
+          <t>3ac0785</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1198,12 +1198,12 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>2025-10-10</t>
+          <t>2025-10-24</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>[•] BUG PERMISOS DE MENUS: se quito el direcionamiento automatico to:/ solo se opto por el @click</t>
+          <t>[] PEPS KARDEX SE AÑADIO FORMA DE VER LOS SALDOS PENDIENTES EN LA TABLA PARA PODER IMPRIMIR</t>
         </is>
       </c>
     </row>
@@ -1213,7 +1213,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>9aeafda</t>
+          <t>62a20fb</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1223,12 +1223,12 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>2025-10-10</t>
+          <t>2025-10-24</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>[•] COMPRA: modificar los btns reposrtes en select</t>
+          <t>[󐊮] INSERTAR: SE INSERTO A COTIZACION PODER LISTAR PUNTOS DE VENTAS SIN CODIGOSIN PARA LOS COMPROBANTES</t>
         </is>
       </c>
     </row>
@@ -1238,7 +1238,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>7790afb</t>
+          <t>10018ef</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1248,12 +1248,12 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>2025-10-10</t>
+          <t>2025-10-23</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>[•] FINALIZACION FACTURA NOTA CREDITO: modificacion backen nota-credito - venta, modificacion front end combinar con contingencia</t>
+          <t>[󐊮] UPDATE KARDEX : se mejoro la consulta a la base de datos y en la api se añadio en el metodo pepes como obtener los precios unitarios y tambien las ventas divididas con diferentes precios por cliente ahora nos toca trabajar en frontend para filtrar de la fecha inicial a la fecha final</t>
         </is>
       </c>
     </row>
@@ -1263,7 +1263,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>613a00f</t>
+          <t>87eb59c</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1273,12 +1273,12 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>2025-10-09</t>
+          <t>2025-10-22</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>[NULL] PENDIENTE KARDEX : solo se quedo en obtner precios de las compras nos falta obtener UEPS PEPS Promedio</t>
+          <t>[󐊮] BUG:no registraba ventas errores que salia es que el ticketFactura ya se habia registrado : error la venta prueba se registraba en impuestos pero no se registraba en mistersoft solucion : se clono ventas para simular que se registraron , se agrego trasabilidad de los extrabios y se registrar el origen en el stock que seria de la compra</t>
         </is>
       </c>
     </row>
@@ -1288,7 +1288,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>4ce76ff</t>
+          <t>429f7b1</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1298,12 +1298,12 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>2025-10-07</t>
+          <t>2025-10-22</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>[●] cambio tarjeta venta inicio a Resgistrar Venta</t>
+          <t>Merge branch 'develop' of https://github.com/aycaRichard12/Ms_comercial into Feacture_Kardex_saldo_inicial_x_lotes_con_saldo marge automatico</t>
         </is>
       </c>
     </row>
@@ -1313,7 +1313,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>332f720</t>
+          <t>79ec238</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1323,12 +1323,12 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>2025-10-07</t>
+          <t>2025-10-22</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>[■] MOD: Configuracion de TITLE PESTAÑA COMERCIAL y AUTOMATICO NOMBRE DE LA EMPRESA</t>
+          <t>Merge branch 'main' of github.com:aycaRichard12/Ms_comercial</t>
         </is>
       </c>
     </row>
@@ -1338,7 +1338,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>28d88a6</t>
+          <t>be2eeca</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1348,12 +1348,12 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>2025-10-07</t>
+          <t>2025-10-22</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>[■] MOD : routes no mostrar rutas solo el link de version</t>
+          <t>[񯢔] CAMBIO EN MAIN BAJARSE EN CADA REPOSITORIO : Se añadio el modal para registrar el punto de vent</t>
         </is>
       </c>
     </row>
@@ -1363,7 +1363,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>d5a9711</t>
+          <t>f6fb50b</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1373,12 +1373,12 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>2025-10-07</t>
+          <t>2025-10-21</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>[■] MOD: Configuracion de TITLE PESTAÑA COMERCIAL y AUTOMATICO NOMBRE DE LA EMPRESA</t>
+          <t>[♦] se añadio trasabilidad en los movimientos de los productos esta en revision si funciona o hay conflicto con otras funciones</t>
         </is>
       </c>
     </row>
@@ -1388,7 +1388,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>7d8f950</t>
+          <t>66c4346</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1398,12 +1398,12 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>2025-10-07</t>
+          <t>2025-10-21</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>[●] MOD: actualizar tabla despues de registrar credito compra</t>
+          <t>Merge pull request #9 from aycaRichard12/develop</t>
         </is>
       </c>
     </row>
@@ -1413,7 +1413,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>b51fb3d</t>
+          <t>4dcd9af</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1423,12 +1423,12 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>2025-10-07</t>
+          <t>2025-10-21</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>[●] MOD: no permite registrar dos veces para la misma compra</t>
+          <t>[•] funciones para sacar reportes de los commits</t>
         </is>
       </c>
     </row>
@@ -1438,7 +1438,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>d8a4322</t>
+          <t>45fd896</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1448,12 +1448,12 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>2025-10-07</t>
+          <t>2025-10-20</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>[●] MOD: actualizar tabla despues de registrar credito compra</t>
+          <t>Merge pull request #8 from aycaRichard12/Feacture-punto_de_venta_cotizacion_facturacion</t>
         </is>
       </c>
     </row>
@@ -1463,7 +1463,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>8262c38</t>
+          <t>ff5c859</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1473,12 +1473,12 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>2025-10-07</t>
+          <t>2025-10-20</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>[●] MOD: no permite registrar dos veces para la misma compra</t>
+          <t>[•] agregar marge adevelop</t>
         </is>
       </c>
     </row>
@@ -1488,7 +1488,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>cf100a2</t>
+          <t>76114b3</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1498,12 +1498,12 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>2025-10-07</t>
+          <t>2025-10-20</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>[◼︎] MOD: USUARIO DE PRUEBAS</t>
+          <t>Merge pull request #7 from aycaRichard12/Feacture-punto_de_venta_cotizacion_facturacion</t>
         </is>
       </c>
     </row>
@@ -1513,7 +1513,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>b5f2ef7</t>
+          <t>5d0f3c8</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1523,12 +1523,12 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>2025-10-06</t>
+          <t>2025-10-20</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>MOD: arreglar routes</t>
+          <t>[•] Se añadio punto de venta a cotizaion y se muestra en los reportes tanto de venta y cotizacion</t>
         </is>
       </c>
     </row>
@@ -1538,7 +1538,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>3be4789</t>
+          <t>15d5fd2</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1548,12 +1548,12 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>2025-10-06</t>
+          <t>2025-10-20</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>[☺] MOD: REPORTE MERMA Y EXTRAVIO Y SELECT REPORTE</t>
+          <t>[♦] PENDIENTE: SE AGREGO PUNTO DE VENTA A LOS REPORTES DE VENTAY SE REGISTRA EL PUNTO DE VENTA EN CADA COTIZACION Y SE ESTA VIENDO COLOCAR EL PUNTO DE VENTA EN LOS REPOSRTE Y FALTA REGISTRO DE ALMACEN</t>
         </is>
       </c>
     </row>
@@ -1563,7 +1563,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>5a87c4c</t>
+          <t>36e9e6d</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1573,12 +1573,12 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>2025-10-06</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>MOD: arreglar routes</t>
+          <t>Merge pull request #6 from aycaRichard12/develop</t>
         </is>
       </c>
     </row>
@@ -1588,7 +1588,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>fef5258</t>
+          <t>da93671</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1598,12 +1598,12 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>2025-10-06</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>[☺] MOD: REPORTE MERMA Y EXTRAVIO Y SELECT REPORTE</t>
+          <t>Merge pull request #5 from aycaRichard12/Feacture-Cotizacion_Detalle_Adicional_Cotizacion</t>
         </is>
       </c>
     </row>
@@ -1613,7 +1613,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>fd450ca</t>
+          <t>0b50aa7</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1623,12 +1623,12 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>2025-10-04</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>eliminar de routes inventarios kardexPage</t>
+          <t>[•] GOOD: se añadio descripcion adicional a cotizacion preferencial o normal en carrito para especificar los servicios tambien se añadio numero factura o ducumento a cotizaion tambien se muestra en los reportes dichos cambios</t>
         </is>
       </c>
     </row>
@@ -1638,7 +1638,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>991ae7c</t>
+          <t>d5cf671</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -1648,12 +1648,12 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>2025-10-04</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>eliminar de routes inventarios kardexPage</t>
+          <t>Merge pull request #4 from aycaRichard12/develop</t>
         </is>
       </c>
     </row>
@@ -1663,7 +1663,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>67469e9</t>
+          <t>feb7ab7</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -1673,12 +1673,12 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>2025-10-04</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>[☺] Mod : cerrar modal (registrar usuario responsable) despues de registrar - cambiar label btn de guardar por aprobado</t>
+          <t>Merge pull request #3 from aycaRichard12/Feacture-Detalle_Venta_Cotizacion</t>
         </is>
       </c>
     </row>
@@ -1688,7 +1688,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>4afec30</t>
+          <t>0225d73</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -1698,12 +1698,12 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>2025-10-04</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>[■] MOD .env para develop</t>
+          <t>[•] Se agrego descripcion adicional en carrito fenta finalizado</t>
         </is>
       </c>
     </row>
@@ -1713,7 +1713,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>a5e2ba8</t>
+          <t>89d2b1b</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -1723,12 +1723,12 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>2025-10-04</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>[☺] Mod : cerrar modal (registrar usuario responsable) despues de registrar - cambiar label btn de guardar por aprobado</t>
+          <t>[•] Se añadio descripcion adicional en carrito ventas debajo de descripcion del producto</t>
         </is>
       </c>
     </row>
@@ -1738,7 +1738,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>51f047d</t>
+          <t>2caed0c</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -1748,12 +1748,12 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>2025-10-04</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>[○] -&gt; Mod Filtrado precio sugerido, Filtrado costo unitaro DC : fitrar a inicio</t>
+          <t>[◘] DEJAR DE RASTREAR .ENV EN DEVELOP</t>
         </is>
       </c>
     </row>
@@ -1763,7 +1763,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>bef63cc</t>
+          <t>21063fe</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -1773,12 +1773,12 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>2025-10-04</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>[○] -&gt; Mod Filtrado precio sugerido, Filtrado costo unitaro DC : fitrar a inicio</t>
+          <t>[◘] DEJAR DE RASTREAR EL .ENV</t>
         </is>
       </c>
     </row>
@@ -1788,7 +1788,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>0d3e4c2</t>
+          <t>3f1f7ca</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -1798,12 +1798,12 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>2025-10-04</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>[■] configuracion develop terminada - estructura usuarios de pruebas - quasar config</t>
+          <t>Merge branch 'main' of https://github.com/aycaRichard12/Ms_comercial</t>
         </is>
       </c>
     </row>
@@ -1813,7 +1813,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>b14e001</t>
+          <t>a70e993</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -1823,12 +1823,12 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>2025-10-03</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>cambio axios + .nev para produccion, mod services con .env, mod usuarios para pruebas locales y produccion, mod credeciales usuarios para inicialisar en desarrollo no afecta a produccion</t>
+          <t>[♦♦] CONFIG: gitignore</t>
         </is>
       </c>
     </row>
@@ -1838,7 +1838,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>99c04fd</t>
+          <t>3b8119a</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -1848,12 +1848,12 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>2025-10-03</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>cambios .env si se subira al git no se ignorara</t>
+          <t>Merge pull request #2 from aycaRichard12/develop</t>
         </is>
       </c>
     </row>
@@ -1863,7 +1863,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>91897d7</t>
+          <t>ac09b1b</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -1873,12 +1873,12 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>2025-10-03</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>configuraicion develop .env, configuracion axios api, confg de services apis externas -&gt; servidor de prueva para hacer lo minimos cambios</t>
+          <t>Merge branch 'main' into develop</t>
         </is>
       </c>
     </row>
@@ -1888,7 +1888,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>67b9aa5</t>
+          <t>8c87406</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -1898,12 +1898,12 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>2025-10-03</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>hacer cambios reporte cuentas por cobrar al generar reporte scroll se posiciona en tabla, añadir kardex a select reportes comiezo de git con ramas</t>
+          <t>Merge pull request #1 from aycaRichard12/Feacture-kardex</t>
         </is>
       </c>
     </row>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>62dbbab</t>
+          <t>40d7dc7</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -1923,12 +1923,12 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>2025-10-02</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>correcciones comercial</t>
+          <t>Merge branch 'develop' of https://github.com/aycaRichard12/Ms_comercial into Feacture-kardex</t>
         </is>
       </c>
     </row>
@@ -1938,7 +1938,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>3e0caaa</t>
+          <t>8627407</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -1948,12 +1948,12 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>2025-09-19</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>cambios comercial -NO SE TERMINO COMERCIAL- -se hizo cambios menus falta terminar reportes-</t>
+          <t>[•] Completado editar saldos eliminar y modal desplegable de los saldos de un producto seleccionado</t>
         </is>
       </c>
     </row>
@@ -1963,7 +1963,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>3a1565d</t>
+          <t>b1c23da</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -1973,12 +1973,12 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>2025-09-16</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>desarrollo ota deito credito</t>
+          <t>[♦] BUG MENU: se aumento en la funcion selectSubmenu otro else if para validar que si no tiene paginas el submenu entonces enrutar a la base del menu</t>
         </is>
       </c>
     </row>
@@ -1988,7 +1988,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>412b529</t>
+          <t>2578a08</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -1998,12 +1998,12 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>2025-09-11</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>Commmit : Solucion de Error Devolucion Venta / mejora de reportes de Venta Gris</t>
+          <t>[•] BUG: correccion bug componente venta se mostraba a inicio sesion apezar de que no tenia permisos para mostrar</t>
         </is>
       </c>
     </row>
@@ -2013,7 +2013,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>7cd7d32</t>
+          <t>92c2751</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -2023,12 +2023,12 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>2025-09-10</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>Api Compra Out y Diseño Estructura Guias Interfaz Quasar y Dirver</t>
+          <t>[♦] BUG MENU: se aumento en la funcion selectSubmenu otro else if para validar que si no tiene paginas el submenu entonces enrutar a la base del menu</t>
         </is>
       </c>
     </row>
@@ -2038,7 +2038,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>a449083</t>
+          <t>af8a9eb</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -2048,12 +2048,12 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>2025-09-09</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>Api out ventas finalzida con los parametros optimizados</t>
+          <t>[•] Iyeccion mistersoft esta fallando venta</t>
         </is>
       </c>
     </row>
@@ -2063,7 +2063,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>b451274</t>
+          <t>bd7bea8</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -2073,12 +2073,12 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>2025-09-03</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>compra creditos</t>
+          <t>[♦] Imcompleto cardex para mostrar detalle de saldo final</t>
         </is>
       </c>
     </row>
@@ -2088,7 +2088,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>dd40fa0</t>
+          <t>d331fac</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -2098,12 +2098,12 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>2025-09-02</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>m:correcciones comercial</t>
+          <t>[♦] PENDIENTE KARDEX: se logro obtener el precio unitario de cada compra y su respectivo movimiento los negativos son salidas y los positivos son movimientos</t>
         </is>
       </c>
     </row>
@@ -2113,7 +2113,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>da37a18</t>
+          <t>0a097e1</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -2123,12 +2123,12 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>2025-08-30</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>Cambios Sistema correcciones primera interacion</t>
+          <t>[•] BUG: correccion bug componente venta se mostraba a inicio sesion apezar de que no tenia permisos para mostrar</t>
         </is>
       </c>
     </row>
@@ -2138,7 +2138,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>f5c4d75</t>
+          <t>7a5032d</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -2148,12 +2148,12 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>2025-08-01</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>Cambios interfaz</t>
+          <t>[♦] IMCOMPLETO: NO SE TERMINO KARDEX</t>
         </is>
       </c>
     </row>
@@ -2163,7 +2163,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>283842d</t>
+          <t>85ed0f8</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -2173,12 +2173,12 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>2025-06-19</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>Eliminar vendor del repo y agregarlo al .gitignore</t>
+          <t>[•] BUG: correccion bug componente venta se mostraba a inicio sesion apezar de que no tenia permisos para mostrar</t>
         </is>
       </c>
     </row>
@@ -2188,7 +2188,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>3501c4e</t>
+          <t>1531505</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -2198,12 +2198,12 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>2025-04-21</t>
+          <t>2025-10-10</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>first commit</t>
+          <t>[•] BUG PERMISOS DE MENUS: se quito el direcionamiento automatico to:/ solo se opto por el @click</t>
         </is>
       </c>
     </row>
@@ -2213,20 +2213,1145 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
+          <t>5b580ba</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>aycaRichard12</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>2025-10-10</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>[•] COMPRA: modificar los btns reposrtes en select</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>71</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>9f1a936</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>aycaRichard12</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>2025-10-10</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>[•] FINALIZACION FACTURA NOTA CREDITO: modificacion backen nota-credito - venta, modificacion front end combinar con contingencia</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>72</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>6faad43</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>aycaRichard12</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>2025-10-07</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>[●] cambio tarjeta venta inicio a Resgistrar Venta</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>73</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>bad185c</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>aycaRichard12</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>2025-10-10</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>[•] BUG PERMISOS DE MENUS: se quito el direcionamiento automatico to:/ solo se opto por el @click</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>74</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>e285b72</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>aycaRichard12</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>2025-10-10</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>[•] BUG PERMISOS DE MENUS: se quito el direcionamiento automatico to:/ solo se opto por el @click</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>75</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>9aeafda</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>aycaRichard12</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>2025-10-10</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>[•] COMPRA: modificar los btns reposrtes en select</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>76</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>7790afb</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>aycaRichard12</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>2025-10-10</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>[•] FINALIZACION FACTURA NOTA CREDITO: modificacion backen nota-credito - venta, modificacion front end combinar con contingencia</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>77</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>613a00f</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>aycaRichard12</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>2025-10-09</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>[NULL] PENDIENTE KARDEX : solo se quedo en obtner precios de las compras nos falta obtener UEPS PEPS Promedio</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>78</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>4ce76ff</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>aycaRichard12</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>2025-10-07</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>[●] cambio tarjeta venta inicio a Resgistrar Venta</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>79</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>332f720</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>aycaRichard12</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>2025-10-07</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>[■] MOD: Configuracion de TITLE PESTAÑA COMERCIAL y AUTOMATICO NOMBRE DE LA EMPRESA</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>80</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>28d88a6</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>aycaRichard12</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>2025-10-07</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>[■] MOD : routes no mostrar rutas solo el link de version</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>81</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>d5a9711</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>aycaRichard12</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>2025-10-07</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>[■] MOD: Configuracion de TITLE PESTAÑA COMERCIAL y AUTOMATICO NOMBRE DE LA EMPRESA</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>82</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>7d8f950</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>aycaRichard12</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>2025-10-07</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>[●] MOD: actualizar tabla despues de registrar credito compra</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>83</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>b51fb3d</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>aycaRichard12</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>2025-10-07</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>[●] MOD: no permite registrar dos veces para la misma compra</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>84</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>d8a4322</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>aycaRichard12</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>2025-10-07</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>[●] MOD: actualizar tabla despues de registrar credito compra</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>85</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>8262c38</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>aycaRichard12</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>2025-10-07</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>[●] MOD: no permite registrar dos veces para la misma compra</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>86</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>cf100a2</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>aycaRichard12</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>2025-10-07</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>[◼︎] MOD: USUARIO DE PRUEBAS</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>87</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>b5f2ef7</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>aycaRichard12</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>2025-10-06</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>MOD: arreglar routes</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>88</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>3be4789</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>aycaRichard12</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>2025-10-06</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>[☺] MOD: REPORTE MERMA Y EXTRAVIO Y SELECT REPORTE</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>89</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>5a87c4c</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>aycaRichard12</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>2025-10-06</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>MOD: arreglar routes</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>90</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>fef5258</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>aycaRichard12</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>2025-10-06</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>[☺] MOD: REPORTE MERMA Y EXTRAVIO Y SELECT REPORTE</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>91</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>fd450ca</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>aycaRichard12</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>2025-10-04</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>eliminar de routes inventarios kardexPage</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>92</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>991ae7c</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>aycaRichard12</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>2025-10-04</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>eliminar de routes inventarios kardexPage</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>93</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>67469e9</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>aycaRichard12</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>2025-10-04</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>[☺] Mod : cerrar modal (registrar usuario responsable) despues de registrar - cambiar label btn de guardar por aprobado</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>94</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>4afec30</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>aycaRichard12</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>2025-10-04</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>[■] MOD .env para develop</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>95</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>a5e2ba8</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>aycaRichard12</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>2025-10-04</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>[☺] Mod : cerrar modal (registrar usuario responsable) despues de registrar - cambiar label btn de guardar por aprobado</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>96</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>51f047d</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>aycaRichard12</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>2025-10-04</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>[○] -&gt; Mod Filtrado precio sugerido, Filtrado costo unitaro DC : fitrar a inicio</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>97</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>bef63cc</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>aycaRichard12</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>2025-10-04</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>[○] -&gt; Mod Filtrado precio sugerido, Filtrado costo unitaro DC : fitrar a inicio</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>98</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>0d3e4c2</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>aycaRichard12</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>2025-10-04</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>[■] configuracion develop terminada - estructura usuarios de pruebas - quasar config</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>99</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>b14e001</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>aycaRichard12</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>2025-10-03</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>cambio axios + .nev para produccion, mod services con .env, mod usuarios para pruebas locales y produccion, mod credeciales usuarios para inicialisar en desarrollo no afecta a produccion</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="n">
+        <v>100</v>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>99c04fd</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>aycaRichard12</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>2025-10-03</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>cambios .env si se subira al git no se ignorara</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="n">
+        <v>101</v>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>91897d7</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>aycaRichard12</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>2025-10-03</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>configuraicion develop .env, configuracion axios api, confg de services apis externas -&gt; servidor de prueva para hacer lo minimos cambios</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="n">
+        <v>102</v>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>67b9aa5</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>aycaRichard12</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>2025-10-03</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>hacer cambios reporte cuentas por cobrar al generar reporte scroll se posiciona en tabla, añadir kardex a select reportes comiezo de git con ramas</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="n">
+        <v>103</v>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>62dbbab</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>aycaRichard12</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>2025-10-02</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>correcciones comercial</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="n">
+        <v>104</v>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>3e0caaa</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>aycaRichard12</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>2025-09-19</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>cambios comercial -NO SE TERMINO COMERCIAL- -se hizo cambios menus falta terminar reportes-</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="n">
+        <v>105</v>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>3a1565d</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>aycaRichard12</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>2025-09-16</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>desarrollo ota deito credito</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="n">
+        <v>106</v>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>412b529</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>aycaRichard12</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>2025-09-11</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>Commmit : Solucion de Error Devolucion Venta / mejora de reportes de Venta Gris</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="n">
+        <v>107</v>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>7cd7d32</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>aycaRichard12</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>2025-09-10</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>Api Compra Out y Diseño Estructura Guias Interfaz Quasar y Dirver</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="n">
+        <v>108</v>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>a449083</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>aycaRichard12</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>2025-09-09</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>Api out ventas finalzida con los parametros optimizados</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="n">
+        <v>109</v>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>b451274</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>aycaRichard12</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>2025-09-03</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>compra creditos</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="n">
+        <v>110</v>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>dd40fa0</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>aycaRichard12</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>2025-09-02</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>m:correcciones comercial</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="n">
+        <v>111</v>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>da37a18</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>aycaRichard12</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>2025-08-30</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>Cambios Sistema correcciones primera interacion</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="n">
+        <v>112</v>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>f5c4d75</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>aycaRichard12</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>2025-08-01</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>Cambios interfaz</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="n">
+        <v>113</v>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>283842d</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>aycaRichard12</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>2025-06-19</t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>Eliminar vendor del repo y agregarlo al .gitignore</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="n">
+        <v>114</v>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>3501c4e</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>aycaRichard12</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>2025-04-21</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>first commit</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="n">
+        <v>115</v>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
           <t>9409db8</t>
         </is>
       </c>
-      <c r="C72" t="inlineStr">
+      <c r="C117" t="inlineStr">
         <is>
           <t>Ricahrd Ayca</t>
         </is>
       </c>
-      <c r="D72" t="inlineStr">
+      <c r="D117" t="inlineStr">
         <is>
           <t>2025-04-01</t>
         </is>
       </c>
-      <c r="E72" t="inlineStr">
+      <c r="E117" t="inlineStr">
         <is>
           <t>Initialize the project 🚀</t>
         </is>

</xml_diff>

<commit_message>
feat(soft externos backend): se añadio la api para software externos el sistema para notificaciones
</commit_message>
<xml_diff>
--- a/reporte_avance.xlsx
+++ b/reporte_avance.xlsx
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E172"/>
+  <dimension ref="A1:E181"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -488,7 +488,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>6a0b405</t>
+          <t>24c46db</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -498,12 +498,12 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>docs(partial-merge): como traer solo commits especificos de otro repositorio</t>
+          <t>refactor(dialog-eliminar): agregar mensaje de eliminacion Creacion Almacen</t>
         </is>
       </c>
     </row>
@@ -513,7 +513,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>806d175</t>
+          <t>45ab8b5</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -523,12 +523,12 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>build(commitizen): herramienta que ayuda a estandarizar los mensajes de commits en git</t>
+          <t>refactor(detalle compra): modificar posicionamiento del simboo divisa</t>
         </is>
       </c>
     </row>
@@ -538,7 +538,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>8f99a94</t>
+          <t>3511926</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -548,12 +548,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>docs(git-commits): guia de commits Profecionales Estructura recomendables en md</t>
+          <t>refactor(p.-precio-sugerido): modificar tabla add column medida x prod simb divisa en col cabezera</t>
         </is>
       </c>
     </row>
@@ -563,7 +563,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>efc80fc</t>
+          <t>dcebd18</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -573,12 +573,12 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>docs(git-remotes) documentacion git agregar repositorios remotos al repositorio principal</t>
+          <t>refactor(p.-cunitario): modificar tabla añadir columna medida x producto divisa en colm cabezera</t>
         </is>
       </c>
     </row>
@@ -588,7 +588,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>143732c</t>
+          <t>7e31079</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -598,12 +598,12 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>fix(responsable-almacen) retornar Almacenes activos asignado y activos e inactivos : se corrigio el use store por que solo se listaba activos e inactivos , se ejecuta otro enpoint para retornar las dos listas sindo uno para nuevos registro como ventas solo los activos, la otra lista es mas para los reportes si antes estuvo activo pero se inavilito sus reportes son necesarios aunque ya esten inactivos</t>
+          <t>refactor(api-configuracion-precios): retornar unidad de medida enpoint p Sugerido y unitario</t>
         </is>
       </c>
     </row>
@@ -613,7 +613,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>b60d003</t>
+          <t>129fd26</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -623,12 +623,12 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2025-12-18</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>chore(routes): Configuracion rutas el historial del router segun entorno (SRC/SPA) Y modo (history / hash)</t>
+          <t>fix(proveedores): modificar btns aliniacion</t>
         </is>
       </c>
     </row>
@@ -638,7 +638,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>ad36443</t>
+          <t>36ee89c</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -648,12 +648,12 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Se mejoro la funcion UseAlmacenStore para devolver las dos respuesta de dos empoints que son endpoint1 = listaResponsableAlmacenReportes/ endpoint2 = listaResponsableAlmacen/</t>
+          <t>chore(pusher): servicio en la nube para gestionar conexciones con las notificaciones</t>
         </is>
       </c>
     </row>
@@ -663,7 +663,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>8b9182f</t>
+          <t>0b6042e</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -673,12 +673,12 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>finalizar filtrado Cuentas por cobrar con filtrado individual por columna con condicionales</t>
+          <t>info(rep-Nov-Dic): reporte avances</t>
         </is>
       </c>
     </row>
@@ -688,7 +688,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>c9fa064</t>
+          <t>70193f8</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -698,12 +698,12 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2025-12-16</t>
+          <t>2025-12-19</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Registrar Credito Cotizacion, tabla armar qr en la tabla</t>
+          <t>docs(mc4-pusher): socket para notificaciones</t>
         </is>
       </c>
     </row>
@@ -713,7 +713,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>a49df34</t>
+          <t>6a0b405</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -723,12 +723,12 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Cambiar Registrar Categoria Precio a submenu Creacion</t>
+          <t>docs(partial-merge): como traer solo commits especificos de otro repositorio</t>
         </is>
       </c>
     </row>
@@ -738,7 +738,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>66aafa6</t>
+          <t>806d175</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -748,12 +748,12 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2025-12-15</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Asignar Categoria Precio a almacen, agregar credito Cotizacion</t>
+          <t>build(commitizen): herramienta que ayuda a estandarizar los mensajes de commits en git</t>
         </is>
       </c>
     </row>
@@ -763,7 +763,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>4eae866</t>
+          <t>8f99a94</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -773,12 +773,12 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Arreglar Facturacion descuentos, Reportes estilo Excel mejorar los get columnas</t>
+          <t>docs(git-commits): guia de commits Profecionales Estructura recomendables en md</t>
         </is>
       </c>
     </row>
@@ -788,7 +788,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2bec562</t>
+          <t>efc80fc</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -798,12 +798,12 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>2025-12-08</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Filtracion implementado en reportes gestion Ventas, Gestion Cotizacion</t>
+          <t>docs(git-remotes) documentacion git agregar repositorios remotos al repositorio principal</t>
         </is>
       </c>
     </row>
@@ -813,7 +813,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>f5be112</t>
+          <t>143732c</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -823,12 +823,12 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Se arreglo el filtrado de los almacenes y se implemento para filtrado general</t>
+          <t>fix(responsable-almacen) retornar Almacenes activos asignado y activos e inactivos : se corrigio el use store por que solo se listaba activos e inactivos , se ejecuta otro enpoint para retornar las dos listas sindo uno para nuevos registro como ventas solo los activos, la otra lista es mas para los reportes si antes estuvo activo pero se inavilito sus reportes son necesarios aunque ya esten inactivos</t>
         </is>
       </c>
     </row>
@@ -838,7 +838,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>75a8bec</t>
+          <t>b60d003</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -848,12 +848,12 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-18</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Merge branch 'main' of github.com:aycaRichard12/Ms_comercial</t>
+          <t>chore(routes): Configuracion rutas el historial del router segun entorno (SRC/SPA) Y modo (history / hash)</t>
         </is>
       </c>
     </row>
@@ -863,7 +863,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>16f3326</t>
+          <t>ad36443</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -873,12 +873,12 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Merge pull request #36 from aycaRichard12/develop</t>
+          <t>Se mejoro la funcion UseAlmacenStore para devolver las dos respuesta de dos empoints que son endpoint1 = listaResponsableAlmacenReportes/ endpoint2 = listaResponsableAlmacen/</t>
         </is>
       </c>
     </row>
@@ -888,7 +888,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>b9ab466</t>
+          <t>8b9182f</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -898,12 +898,12 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>listar almacenes activos al hacer una transaccion en compra, venta, cotizacion, merma, extrabio pero en reportes mostrar todos los almacenes, mostrar en detalle compra al añadir un producto al carrito su medida, correcciones comercial en general</t>
+          <t>finalizar filtrado Cuentas por cobrar con filtrado individual por columna con condicionales</t>
         </is>
       </c>
     </row>
@@ -913,7 +913,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>ebb7cf7</t>
+          <t>c9fa064</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -923,12 +923,12 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>2025-12-03</t>
+          <t>2025-12-16</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Se agrego la funcion de cerrar los reportes PDFs con ECS</t>
+          <t>Registrar Credito Cotizacion, tabla armar qr en la tabla</t>
         </is>
       </c>
     </row>
@@ -938,7 +938,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>227f72c</t>
+          <t>a49df34</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -948,12 +948,12 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Anular out Factura</t>
+          <t>Cambiar Registrar Categoria Precio a submenu Creacion</t>
         </is>
       </c>
     </row>
@@ -963,7 +963,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>0f88213</t>
+          <t>66aafa6</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -973,12 +973,12 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-15</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Merge pull request #35 from aycaRichard12/develop</t>
+          <t>Asignar Categoria Precio a almacen, agregar credito Cotizacion</t>
         </is>
       </c>
     </row>
@@ -988,7 +988,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>3318ec5</t>
+          <t>4eae866</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -998,12 +998,12 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>2025-12-02</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>SE QUITO LA VALIDACION DE FACTUA SIN, SE REIMPLANTARA POSTERIORMENTE</t>
+          <t>Arreglar Facturacion descuentos, Reportes estilo Excel mejorar los get columnas</t>
         </is>
       </c>
     </row>
@@ -1013,7 +1013,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>9b469e9</t>
+          <t>2bec562</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1023,12 +1023,12 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-08</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Merge pull request #34 from aycaRichard12/develop</t>
+          <t>Filtracion implementado en reportes gestion Ventas, Gestion Cotizacion</t>
         </is>
       </c>
     </row>
@@ -1038,7 +1038,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>ed0f4b0</t>
+          <t>f5be112</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1048,12 +1048,12 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>desarrollo de devolucion de venta</t>
+          <t>Se arreglo el filtrado de los almacenes y se implemento para filtrado general</t>
         </is>
       </c>
     </row>
@@ -1063,7 +1063,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>7e0f433</t>
+          <t>75a8bec</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1073,12 +1073,12 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Merge pull request #33 from aycaRichard12/develop</t>
+          <t>Merge branch 'main' of github.com:aycaRichard12/Ms_comercial</t>
         </is>
       </c>
     </row>
@@ -1088,7 +1088,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>c9a2aef</t>
+          <t>16f3326</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1098,12 +1098,12 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>2025-12-01</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Correcciones reportes PDF</t>
+          <t>Merge pull request #36 from aycaRichard12/develop</t>
         </is>
       </c>
     </row>
@@ -1113,7 +1113,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>e3ffb9e</t>
+          <t>b9ab466</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1123,12 +1123,12 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Merge pull request #32 from aycaRichard12/develop</t>
+          <t>listar almacenes activos al hacer una transaccion en compra, venta, cotizacion, merma, extrabio pero en reportes mostrar todos los almacenes, mostrar en detalle compra al añadir un producto al carrito su medida, correcciones comercial en general</t>
         </is>
       </c>
     </row>
@@ -1138,7 +1138,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>c8bcf11</t>
+          <t>ebb7cf7</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1148,12 +1148,12 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>2025-11-29</t>
+          <t>2025-12-03</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>correcciones Informe PDFs</t>
+          <t>Se agrego la funcion de cerrar los reportes PDFs con ECS</t>
         </is>
       </c>
     </row>
@@ -1163,7 +1163,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>ac108c7</t>
+          <t>227f72c</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1173,12 +1173,12 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Merge pull request #31 from aycaRichard12/develop</t>
+          <t>Anular out Factura</t>
         </is>
       </c>
     </row>
@@ -1188,7 +1188,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>8ce9d82</t>
+          <t>0f88213</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1198,12 +1198,12 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>[•] modificaciones Reporte modelo PDF</t>
+          <t>Merge pull request #35 from aycaRichard12/develop</t>
         </is>
       </c>
     </row>
@@ -1213,7 +1213,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>1de06f0</t>
+          <t>3318ec5</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1223,12 +1223,12 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-12-02</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Merge pull request #30 from aycaRichard12/develop</t>
+          <t>SE QUITO LA VALIDACION DE FACTUA SIN, SE REIMPLANTARA POSTERIORMENTE</t>
         </is>
       </c>
     </row>
@@ -1238,7 +1238,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>5573204</t>
+          <t>9b469e9</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1248,12 +1248,12 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Merge pull request #29 from aycaRichard12/F_correcciones_comercial</t>
+          <t>Merge pull request #34 from aycaRichard12/develop</t>
         </is>
       </c>
     </row>
@@ -1263,7 +1263,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>45bf567</t>
+          <t>ed0f4b0</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1273,12 +1273,12 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>correcciones Comercial</t>
+          <t>desarrollo de devolucion de venta</t>
         </is>
       </c>
     </row>
@@ -1288,7 +1288,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>5b9ae78</t>
+          <t>7e0f433</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1298,12 +1298,12 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>2025-11-28</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>[•] se agrego el modelo nuevo de reportes PDF general, los reportes que se desarrollo en su propio pagina o componente en un principio mover a reportes global</t>
+          <t>Merge pull request #33 from aycaRichard12/develop</t>
         </is>
       </c>
     </row>
@@ -1313,7 +1313,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>e471fe0</t>
+          <t>c9a2aef</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1323,12 +1323,12 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-12-01</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Merge pull request #28 from aycaRichard12/F_correcciones_comercial</t>
+          <t>Correcciones reportes PDF</t>
         </is>
       </c>
     </row>
@@ -1338,7 +1338,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>ec2d3b7</t>
+          <t>e3ffb9e</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1348,12 +1348,12 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>2025-11-22</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Correcciones cotizacion Facturacion</t>
+          <t>Merge pull request #32 from aycaRichard12/develop</t>
         </is>
       </c>
     </row>
@@ -1363,7 +1363,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>573c017</t>
+          <t>c8bcf11</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1373,12 +1373,12 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>2025-11-21</t>
+          <t>2025-11-29</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>[CORRECCIONES] añadir cabezera en reporte pdf extravio y merma datos del usuario y datos de la merma o extravio con fecha de impresion</t>
+          <t>correcciones Informe PDFs</t>
         </is>
       </c>
     </row>
@@ -1388,7 +1388,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>2ff0646</t>
+          <t>ac108c7</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1398,12 +1398,12 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>2025-11-21</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>[CORRECCIONES] mostrar en reportes mermas y extrabios un modal de los detalles de los productos registrados en caso de un extravio o un robo</t>
+          <t>Merge pull request #31 from aycaRichard12/develop</t>
         </is>
       </c>
     </row>
@@ -1413,7 +1413,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>d157595</t>
+          <t>8ce9d82</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1423,12 +1423,12 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>2025-11-21</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Merge pull request #27 from aycaRichard12/develop</t>
+          <t>[•] modificaciones Reporte modelo PDF</t>
         </is>
       </c>
     </row>
@@ -1438,7 +1438,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>33187f2</t>
+          <t>1de06f0</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1448,12 +1448,12 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>2025-11-21</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Merge pull request #26 from aycaRichard12/F_cotizacion_devolucion</t>
+          <t>Merge pull request #30 from aycaRichard12/develop</t>
         </is>
       </c>
     </row>
@@ -1463,7 +1463,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>8ddc7c5</t>
+          <t>5573204</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1473,12 +1473,12 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>2025-11-21</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>[DEVOLUCION COTIZACION] - ADD DEVOLUCION COTIZACION REGISTRO DE DETALLE DEVOLUCION , AUTORIZACION DE STOCK DEVOLUCION COTIZACION, CAMBIOS REPORTES COTIZACION PARA QUE APARESCA CON ESTADO DEV NO FACTURABLE, VER COTIZACION EN DEVOLUCIONES EN REPORTE CONTINGENCIAS Y PODER VER EN COTIZACIONES, SE AÑADIO EN NOTACREDITODEBITO EL TIPO DE DOCUMENTO QUE ES UNA VENTA FACTURADA</t>
+          <t>Merge pull request #29 from aycaRichard12/F_correcciones_comercial</t>
         </is>
       </c>
     </row>
@@ -1488,7 +1488,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>9fcacac</t>
+          <t>45bf567</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1498,12 +1498,12 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>2025-11-20</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>SE SACO REPORTE PARA INFORME DE AVANCE, SE AÑADIO TIPO DE CAMBIO CON TOTAL</t>
+          <t>correcciones Comercial</t>
         </is>
       </c>
     </row>
@@ -1513,7 +1513,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>c95656c</t>
+          <t>5b9ae78</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1523,12 +1523,12 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>2025-11-18</t>
+          <t>2025-11-28</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>añadir anular Cotizacion en cuentas Sin Factura</t>
+          <t>[•] se agrego el modelo nuevo de reportes PDF general, los reportes que se desarrollo en su propio pagina o componente en un principio mover a reportes global</t>
         </is>
       </c>
     </row>
@@ -1538,7 +1538,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>0b77139</t>
+          <t>e471fe0</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1548,12 +1548,12 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>2025-11-18</t>
+          <t>2025-11-22</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Merge pull request #25 from aycaRichard12/develop</t>
+          <t>Merge pull request #28 from aycaRichard12/F_correcciones_comercial</t>
         </is>
       </c>
     </row>
@@ -1563,7 +1563,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>9763c03</t>
+          <t>ec2d3b7</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1573,12 +1573,12 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>2025-11-18</t>
+          <t>2025-11-22</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>registrar precio sugerido que afecte a todos los almacenes, actulizar tabla compra al registrar automaticamente filtrar del almacen registrodo,visualizar la factura despues de registrar en factura , factura exportacion , factura alquiler, bug mostrar reporte pdf de compras por almacen</t>
+          <t>Correcciones cotizacion Facturacion</t>
         </is>
       </c>
     </row>
@@ -1588,7 +1588,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>650c24d</t>
+          <t>573c017</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1598,12 +1598,12 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>2025-11-17</t>
+          <t>2025-11-21</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Merge pull request #24 from aycaRichard12/develop</t>
+          <t>[CORRECCIONES] añadir cabezera en reporte pdf extravio y merma datos del usuario y datos de la merma o extravio con fecha de impresion</t>
         </is>
       </c>
     </row>
@@ -1613,7 +1613,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>44260ca</t>
+          <t>2ff0646</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1623,12 +1623,12 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>2025-11-17</t>
+          <t>2025-11-21</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>se normalizo useCotizacion que se trajabaron de prueba respuesta de emizor por defecto se quito se añadio el simbolo de moneda en reporte ventas hoy, se añadio eniviar por correo el comprobante o la factura de impuesto tambien al facturar una cotizacion se podra ver la factura despues, se mejoro el reporte para que un link de un pdf sea enviado por correo</t>
+          <t>[CORRECCIONES] mostrar en reportes mermas y extrabios un modal de los detalles de los productos registrados en caso de un extravio o un robo</t>
         </is>
       </c>
     </row>
@@ -1638,7 +1638,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>a136883</t>
+          <t>d157595</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -1648,12 +1648,12 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>2025-11-17</t>
+          <t>2025-11-21</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Merge pull request #23 from aycaRichard12/develop</t>
+          <t>Merge pull request #27 from aycaRichard12/develop</t>
         </is>
       </c>
     </row>
@@ -1663,7 +1663,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>6590116</t>
+          <t>33187f2</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -1673,12 +1673,12 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>2025-11-17</t>
+          <t>2025-11-21</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Arreglar cosigo sin producto, cotizacion facurar de normal y preferencial cambios de estado 2 facturado y no se puede facturar 2 veces</t>
+          <t>Merge pull request #26 from aycaRichard12/F_cotizacion_devolucion</t>
         </is>
       </c>
     </row>
@@ -1688,7 +1688,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>8ab1917</t>
+          <t>8ddc7c5</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -1698,12 +1698,12 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>2025-11-13</t>
+          <t>2025-11-21</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Merge pull request #22 from aycaRichard12/develop</t>
+          <t>[DEVOLUCION COTIZACION] - ADD DEVOLUCION COTIZACION REGISTRO DE DETALLE DEVOLUCION , AUTORIZACION DE STOCK DEVOLUCION COTIZACION, CAMBIOS REPORTES COTIZACION PARA QUE APARESCA CON ESTADO DEV NO FACTURABLE, VER COTIZACION EN DEVOLUCIONES EN REPORTE CONTINGENCIAS Y PODER VER EN COTIZACIONES, SE AÑADIO EN NOTACREDITODEBITO EL TIPO DE DOCUMENTO QUE ES UNA VENTA FACTURADA</t>
         </is>
       </c>
     </row>
@@ -1713,7 +1713,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>b8cc5cb</t>
+          <t>9fcacac</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -1723,12 +1723,12 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>2025-11-13</t>
+          <t>2025-11-20</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>en App se quito la comparacion du usuario</t>
+          <t>SE SACO REPORTE PARA INFORME DE AVANCE, SE AÑADIO TIPO DE CAMBIO CON TOTAL</t>
         </is>
       </c>
     </row>
@@ -1738,7 +1738,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>28f2bf8</t>
+          <t>c95656c</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -1748,12 +1748,12 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>2025-11-13</t>
+          <t>2025-11-18</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Merge pull request #21 from aycaRichard12/develop</t>
+          <t>añadir anular Cotizacion en cuentas Sin Factura</t>
         </is>
       </c>
     </row>
@@ -1763,7 +1763,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>25a40d2</t>
+          <t>0b77139</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -1773,12 +1773,12 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>2025-11-13</t>
+          <t>2025-11-18</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Cambios Factura Exportacion add tipo cambio dinamico</t>
+          <t>Merge pull request #25 from aycaRichard12/develop</t>
         </is>
       </c>
     </row>
@@ -1788,7 +1788,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>63d4433</t>
+          <t>9763c03</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -1798,12 +1798,12 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>2025-11-13</t>
+          <t>2025-11-18</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>cotizacion facturar cotizacion Normal , arreglo facturacion Comercializacion</t>
+          <t>registrar precio sugerido que afecte a todos los almacenes, actulizar tabla compra al registrar automaticamente filtrar del almacen registrodo,visualizar la factura despues de registrar en factura , factura exportacion , factura alquiler, bug mostrar reporte pdf de compras por almacen</t>
         </is>
       </c>
     </row>
@@ -1813,7 +1813,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>b74c208</t>
+          <t>650c24d</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -1823,12 +1823,12 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>2025-11-10</t>
+          <t>2025-11-17</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>Merge pull request #20 from aycaRichard12/develop</t>
+          <t>Merge pull request #24 from aycaRichard12/develop</t>
         </is>
       </c>
     </row>
@@ -1838,7 +1838,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>c07fefa</t>
+          <t>44260ca</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -1848,12 +1848,12 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>2025-11-08</t>
+          <t>2025-11-17</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>comando por voz, correcciones comercial interfaz , se añadio filtro excel en almacen</t>
+          <t>se normalizo useCotizacion que se trajabaron de prueba respuesta de emizor por defecto se quito se añadio el simbolo de moneda en reporte ventas hoy, se añadio eniviar por correo el comprobante o la factura de impuesto tambien al facturar una cotizacion se podra ver la factura despues, se mejoro el reporte para que un link de un pdf sea enviado por correo</t>
         </is>
       </c>
     </row>
@@ -1863,7 +1863,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>b143628</t>
+          <t>a136883</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -1873,12 +1873,12 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>2025-11-06</t>
+          <t>2025-11-17</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>Merge pull request #19 from aycaRichard12/develop</t>
+          <t>Merge pull request #23 from aycaRichard12/develop</t>
         </is>
       </c>
     </row>
@@ -1888,7 +1888,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>c81402a</t>
+          <t>6590116</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -1898,12 +1898,12 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>2025-11-06</t>
+          <t>2025-11-17</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>Se arreglo cambio de estado merma</t>
+          <t>Arreglar cosigo sin producto, cotizacion facurar de normal y preferencial cambios de estado 2 facturado y no se puede facturar 2 veces</t>
         </is>
       </c>
     </row>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>3004e31</t>
+          <t>8ab1917</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -1923,12 +1923,12 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>2025-11-06</t>
+          <t>2025-11-13</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>Se arreglo cambio de estado robo</t>
+          <t>Merge pull request #22 from aycaRichard12/develop</t>
         </is>
       </c>
     </row>
@@ -1938,7 +1938,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>4218a69</t>
+          <t>b8cc5cb</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -1948,12 +1948,12 @@
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>2025-11-06</t>
+          <t>2025-11-13</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>Merge pull request #18 from aycaRichard12/develop</t>
+          <t>en App se quito la comparacion du usuario</t>
         </is>
       </c>
     </row>
@@ -1963,7 +1963,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>2472148</t>
+          <t>28f2bf8</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -1973,12 +1973,12 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>2025-11-06</t>
+          <t>2025-11-13</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>[•] Añadir cambios anulacion cotizacion, pdf con sangria Anulado, fitrado tabla similar excel</t>
+          <t>Merge pull request #21 from aycaRichard12/develop</t>
         </is>
       </c>
     </row>
@@ -1988,7 +1988,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>3c3f990</t>
+          <t>25a40d2</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -1998,12 +1998,12 @@
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>2025-11-01</t>
+          <t>2025-11-13</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>Se Actualizo bugs de errores de cotizacion como por ejemplo estado solo hay dos 0 y 1 que significa NORMAL y PREFERENCIAL y se añadio en la base de datos una columna condicion para ver si esta activa o anulada la cotizacion se realizo las pruebas respectivas, se separo la logica en 2 variables estado y condicion</t>
+          <t>Cambios Factura Exportacion add tipo cambio dinamico</t>
         </is>
       </c>
     </row>
@@ -2013,7 +2013,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>be62e5c</t>
+          <t>63d4433</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -2023,12 +2023,12 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>2025-10-31</t>
+          <t>2025-11-13</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>Merge pull request #17 from aycaRichard12/Feacture-Anulacion-Cotizacion</t>
+          <t>cotizacion facturar cotizacion Normal , arreglo facturacion Comercializacion</t>
         </is>
       </c>
     </row>
@@ -2038,7 +2038,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>5a0ab7a</t>
+          <t>b74c208</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -2048,12 +2048,12 @@
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>2025-10-31</t>
+          <t>2025-11-10</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>[•] ANULAR COTIZACION DE COMERCIAL, MOSTRAR EN PDF ESPECIFICAMENTE EL DOCUMENTO ANULADO LA SANGRIA</t>
+          <t>Merge pull request #20 from aycaRichard12/develop</t>
         </is>
       </c>
     </row>
@@ -2063,7 +2063,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>e451dc9</t>
+          <t>c07fefa</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -2073,12 +2073,12 @@
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>2025-10-30</t>
+          <t>2025-11-08</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>Merge branch 'main' of github.com:aycaRichard12/Ms_comercial</t>
+          <t>comando por voz, correcciones comercial interfaz , se añadio filtro excel en almacen</t>
         </is>
       </c>
     </row>
@@ -2088,7 +2088,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>2fa385f</t>
+          <t>b143628</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -2098,12 +2098,12 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>2025-10-30</t>
+          <t>2025-11-06</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>[•] Configuracion Inicial</t>
+          <t>Merge pull request #19 from aycaRichard12/develop</t>
         </is>
       </c>
     </row>
@@ -2113,7 +2113,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>a26a606</t>
+          <t>c81402a</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -2123,12 +2123,12 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>2025-10-30</t>
+          <t>2025-11-06</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>Merge pull request #16 from aycaRichard12/develop</t>
+          <t>Se arreglo cambio de estado merma</t>
         </is>
       </c>
     </row>
@@ -2138,7 +2138,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>e40fe0e</t>
+          <t>3004e31</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -2148,12 +2148,12 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>2025-10-30</t>
+          <t>2025-11-06</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>Merge pull request #15 from aycaRichard12/Feacture-Anulacion-Cotizacion</t>
+          <t>Se arreglo cambio de estado robo</t>
         </is>
       </c>
     </row>
@@ -2163,7 +2163,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>e5209e4</t>
+          <t>4218a69</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -2173,12 +2173,12 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>2025-10-30</t>
+          <t>2025-11-06</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>[•] Añadir la opcion de que sea opcional el especificar el lote de la compra al registrar ROBOS y MERMAS</t>
+          <t>Merge pull request #18 from aycaRichard12/develop</t>
         </is>
       </c>
     </row>
@@ -2188,7 +2188,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>1175a19</t>
+          <t>2472148</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -2198,12 +2198,12 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>2025-10-29</t>
+          <t>2025-11-06</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>Merge pull request #14 from aycaRichard12/Feacture-Correcciones</t>
+          <t>[•] Añadir cambios anulacion cotizacion, pdf con sangria Anulado, fitrado tabla similar excel</t>
         </is>
       </c>
     </row>
@@ -2213,7 +2213,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>bdef3d7</t>
+          <t>3c3f990</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -2223,12 +2223,12 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>2025-10-29</t>
+          <t>2025-11-01</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>[•] botones asignar almacen alineados en fila</t>
+          <t>Se Actualizo bugs de errores de cotizacion como por ejemplo estado solo hay dos 0 y 1 que significa NORMAL y PREFERENCIAL y se añadio en la base de datos una columna condicion para ver si esta activa o anulada la cotizacion se realizo las pruebas respectivas, se separo la logica en 2 variables estado y condicion</t>
         </is>
       </c>
     </row>
@@ -2238,7 +2238,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>4c4c7c6</t>
+          <t>be62e5c</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -2248,12 +2248,12 @@
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>2025-10-29</t>
+          <t>2025-10-31</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>[•] Crear titulos para asignar almacen asignar punto de venta y asignar productos</t>
+          <t>Merge pull request #17 from aycaRichard12/Feacture-Anulacion-Cotizacion</t>
         </is>
       </c>
     </row>
@@ -2263,7 +2263,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>5aac9fd</t>
+          <t>5a0ab7a</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -2273,12 +2273,12 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>2025-10-29</t>
+          <t>2025-10-31</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>[•] Colocar Iconos a paginas de pedidos</t>
+          <t>[•] ANULAR COTIZACION DE COMERCIAL, MOSTRAR EN PDF ESPECIFICAMENTE EL DOCUMENTO ANULADO LA SANGRIA</t>
         </is>
       </c>
     </row>
@@ -2288,7 +2288,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>f45fc46</t>
+          <t>e451dc9</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -2298,12 +2298,12 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>2025-10-29</t>
+          <t>2025-10-30</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>[•] Etiquetas a botones de MOvimientos cambiar icon de carrito</t>
+          <t>Merge branch 'main' of github.com:aycaRichard12/Ms_comercial</t>
         </is>
       </c>
     </row>
@@ -2313,7 +2313,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>d87b7cf</t>
+          <t>2fa385f</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -2323,12 +2323,12 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>2025-10-29</t>
+          <t>2025-10-30</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>[•] Movimientos muestra de forma ordenada columna N°</t>
+          <t>[•] Configuracion Inicial</t>
         </is>
       </c>
     </row>
@@ -2338,7 +2338,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>553336b</t>
+          <t>a26a606</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -2348,12 +2348,12 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>2025-10-29</t>
+          <t>2025-10-30</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>Merge pull request #13 from aycaRichard12/develop</t>
+          <t>Merge pull request #16 from aycaRichard12/develop</t>
         </is>
       </c>
     </row>
@@ -2363,7 +2363,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>d661372</t>
+          <t>e40fe0e</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -2373,12 +2373,12 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>2025-10-29</t>
+          <t>2025-10-30</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>[•] Finalizacion obtener token del emizor para la venta out</t>
+          <t>Merge pull request #15 from aycaRichard12/Feacture-Anulacion-Cotizacion</t>
         </is>
       </c>
     </row>
@@ -2388,7 +2388,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>e82f119</t>
+          <t>e5209e4</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -2398,12 +2398,12 @@
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>2025-10-28</t>
+          <t>2025-10-30</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>Merge pull request #12 from aycaRichard12/develop</t>
+          <t>[•] Añadir la opcion de que sea opcional el especificar el lote de la compra al registrar ROBOS y MERMAS</t>
         </is>
       </c>
     </row>
@@ -2413,7 +2413,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>3b28f38</t>
+          <t>1175a19</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -2423,12 +2423,12 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>2025-10-28</t>
+          <t>2025-10-29</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>[•] registrar venta por una ruta diferente en php out/venta metodo POST simplificar endpoint venta para la pagina web ya se hizo la prueba</t>
+          <t>Merge pull request #14 from aycaRichard12/Feacture-Correcciones</t>
         </is>
       </c>
     </row>
@@ -2438,7 +2438,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>dd75382</t>
+          <t>bdef3d7</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -2448,12 +2448,12 @@
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>2025-10-28</t>
+          <t>2025-10-29</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>[•] ACTUALIZAR apis exteriores para comercial y que funciones bien</t>
+          <t>[•] botones asignar almacen alineados en fila</t>
         </is>
       </c>
     </row>
@@ -2463,7 +2463,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>cea6f96</t>
+          <t>4c4c7c6</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -2473,12 +2473,12 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>2025-10-25</t>
+          <t>2025-10-29</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>Merge pull request #11 from aycaRichard12/develop</t>
+          <t>[•] Crear titulos para asignar almacen asignar punto de venta y asignar productos</t>
         </is>
       </c>
     </row>
@@ -2488,7 +2488,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>1dbbaed</t>
+          <t>5aac9fd</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -2498,12 +2498,12 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>2025-10-25</t>
+          <t>2025-10-29</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>Merge pull request #10 from aycaRichard12/Feacture_Kardex_saldo_inicial_x_lotes_con_saldo</t>
+          <t>[•] Colocar Iconos a paginas de pedidos</t>
         </is>
       </c>
     </row>
@@ -2513,7 +2513,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>b182dc3</t>
+          <t>f45fc46</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -2523,12 +2523,12 @@
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>2025-10-25</t>
+          <t>2025-10-29</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>[•] Finalizacion de kardex entrara a rebicion: se modifico el metodo PROMEDIO para hacer las calculos respectivos se arreglo el bug de los reposrtes en pdf</t>
+          <t>[•] Etiquetas a botones de MOvimientos cambiar icon de carrito</t>
         </is>
       </c>
     </row>
@@ -2538,7 +2538,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>07716be</t>
+          <t>d87b7cf</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -2548,12 +2548,12 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>2025-10-24</t>
+          <t>2025-10-29</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>Merge branch 'main' of https://github.com/aycaRichard12/Ms_comercial into Feacture_Kardex_saldo_inicial_x_lotes_con_saldo</t>
+          <t>[•] Movimientos muestra de forma ordenada columna N°</t>
         </is>
       </c>
     </row>
@@ -2563,7 +2563,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>3ac0785</t>
+          <t>553336b</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -2573,12 +2573,12 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>2025-10-24</t>
+          <t>2025-10-29</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>[] PEPS KARDEX SE AÑADIO FORMA DE VER LOS SALDOS PENDIENTES EN LA TABLA PARA PODER IMPRIMIR</t>
+          <t>Merge pull request #13 from aycaRichard12/develop</t>
         </is>
       </c>
     </row>
@@ -2588,7 +2588,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>62a20fb</t>
+          <t>d661372</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -2598,12 +2598,12 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>2025-10-24</t>
+          <t>2025-10-29</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>[󐊮] INSERTAR: SE INSERTO A COTIZACION PODER LISTAR PUNTOS DE VENTAS SIN CODIGOSIN PARA LOS COMPROBANTES</t>
+          <t>[•] Finalizacion obtener token del emizor para la venta out</t>
         </is>
       </c>
     </row>
@@ -2613,7 +2613,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>10018ef</t>
+          <t>e82f119</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -2623,12 +2623,12 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>2025-10-23</t>
+          <t>2025-10-28</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>[󐊮] UPDATE KARDEX : se mejoro la consulta a la base de datos y en la api se añadio en el metodo pepes como obtener los precios unitarios y tambien las ventas divididas con diferentes precios por cliente ahora nos toca trabajar en frontend para filtrar de la fecha inicial a la fecha final</t>
+          <t>Merge pull request #12 from aycaRichard12/develop</t>
         </is>
       </c>
     </row>
@@ -2638,7 +2638,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>87eb59c</t>
+          <t>3b28f38</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -2648,12 +2648,12 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>2025-10-22</t>
+          <t>2025-10-28</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>[󐊮] BUG:no registraba ventas errores que salia es que el ticketFactura ya se habia registrado : error la venta prueba se registraba en impuestos pero no se registraba en mistersoft solucion : se clono ventas para simular que se registraron , se agrego trasabilidad de los extrabios y se registrar el origen en el stock que seria de la compra</t>
+          <t>[•] registrar venta por una ruta diferente en php out/venta metodo POST simplificar endpoint venta para la pagina web ya se hizo la prueba</t>
         </is>
       </c>
     </row>
@@ -2663,7 +2663,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>429f7b1</t>
+          <t>dd75382</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -2673,12 +2673,12 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>2025-10-22</t>
+          <t>2025-10-28</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>Merge branch 'develop' of https://github.com/aycaRichard12/Ms_comercial into Feacture_Kardex_saldo_inicial_x_lotes_con_saldo marge automatico</t>
+          <t>[•] ACTUALIZAR apis exteriores para comercial y que funciones bien</t>
         </is>
       </c>
     </row>
@@ -2688,7 +2688,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>79ec238</t>
+          <t>cea6f96</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -2698,12 +2698,12 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>2025-10-22</t>
+          <t>2025-10-25</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>Merge branch 'main' of github.com:aycaRichard12/Ms_comercial</t>
+          <t>Merge pull request #11 from aycaRichard12/develop</t>
         </is>
       </c>
     </row>
@@ -2713,7 +2713,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>be2eeca</t>
+          <t>1dbbaed</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -2723,12 +2723,12 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>2025-10-22</t>
+          <t>2025-10-25</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>[񯢔] CAMBIO EN MAIN BAJARSE EN CADA REPOSITORIO : Se añadio el modal para registrar el punto de vent</t>
+          <t>Merge pull request #10 from aycaRichard12/Feacture_Kardex_saldo_inicial_x_lotes_con_saldo</t>
         </is>
       </c>
     </row>
@@ -2738,7 +2738,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>f6fb50b</t>
+          <t>b182dc3</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -2748,12 +2748,12 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>2025-10-21</t>
+          <t>2025-10-25</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>[♦] se añadio trasabilidad en los movimientos de los productos esta en revision si funciona o hay conflicto con otras funciones</t>
+          <t>[•] Finalizacion de kardex entrara a rebicion: se modifico el metodo PROMEDIO para hacer las calculos respectivos se arreglo el bug de los reposrtes en pdf</t>
         </is>
       </c>
     </row>
@@ -2763,7 +2763,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>66c4346</t>
+          <t>07716be</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -2773,12 +2773,12 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>2025-10-21</t>
+          <t>2025-10-24</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>Merge pull request #9 from aycaRichard12/develop</t>
+          <t>Merge branch 'main' of https://github.com/aycaRichard12/Ms_comercial into Feacture_Kardex_saldo_inicial_x_lotes_con_saldo</t>
         </is>
       </c>
     </row>
@@ -2788,7 +2788,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>4dcd9af</t>
+          <t>3ac0785</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -2798,12 +2798,12 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>2025-10-21</t>
+          <t>2025-10-24</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>[•] funciones para sacar reportes de los commits</t>
+          <t>[] PEPS KARDEX SE AÑADIO FORMA DE VER LOS SALDOS PENDIENTES EN LA TABLA PARA PODER IMPRIMIR</t>
         </is>
       </c>
     </row>
@@ -2813,7 +2813,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>45fd896</t>
+          <t>62a20fb</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -2823,12 +2823,12 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>2025-10-20</t>
+          <t>2025-10-24</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>Merge pull request #8 from aycaRichard12/Feacture-punto_de_venta_cotizacion_facturacion</t>
+          <t>[󐊮] INSERTAR: SE INSERTO A COTIZACION PODER LISTAR PUNTOS DE VENTAS SIN CODIGOSIN PARA LOS COMPROBANTES</t>
         </is>
       </c>
     </row>
@@ -2838,7 +2838,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>ff5c859</t>
+          <t>10018ef</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -2848,12 +2848,12 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>2025-10-20</t>
+          <t>2025-10-23</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>[•] agregar marge adevelop</t>
+          <t>[󐊮] UPDATE KARDEX : se mejoro la consulta a la base de datos y en la api se añadio en el metodo pepes como obtener los precios unitarios y tambien las ventas divididas con diferentes precios por cliente ahora nos toca trabajar en frontend para filtrar de la fecha inicial a la fecha final</t>
         </is>
       </c>
     </row>
@@ -2863,7 +2863,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>76114b3</t>
+          <t>87eb59c</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -2873,12 +2873,12 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>2025-10-20</t>
+          <t>2025-10-22</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>Merge pull request #7 from aycaRichard12/Feacture-punto_de_venta_cotizacion_facturacion</t>
+          <t>[󐊮] BUG:no registraba ventas errores que salia es que el ticketFactura ya se habia registrado : error la venta prueba se registraba en impuestos pero no se registraba en mistersoft solucion : se clono ventas para simular que se registraron , se agrego trasabilidad de los extrabios y se registrar el origen en el stock que seria de la compra</t>
         </is>
       </c>
     </row>
@@ -2888,7 +2888,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>5d0f3c8</t>
+          <t>429f7b1</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -2898,12 +2898,12 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>2025-10-20</t>
+          <t>2025-10-22</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>[•] Se añadio punto de venta a cotizaion y se muestra en los reportes tanto de venta y cotizacion</t>
+          <t>Merge branch 'develop' of https://github.com/aycaRichard12/Ms_comercial into Feacture_Kardex_saldo_inicial_x_lotes_con_saldo marge automatico</t>
         </is>
       </c>
     </row>
@@ -2913,7 +2913,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>15d5fd2</t>
+          <t>79ec238</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -2923,12 +2923,12 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>2025-10-20</t>
+          <t>2025-10-22</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>[♦] PENDIENTE: SE AGREGO PUNTO DE VENTA A LOS REPORTES DE VENTAY SE REGISTRA EL PUNTO DE VENTA EN CADA COTIZACION Y SE ESTA VIENDO COLOCAR EL PUNTO DE VENTA EN LOS REPOSRTE Y FALTA REGISTRO DE ALMACEN</t>
+          <t>Merge branch 'main' of github.com:aycaRichard12/Ms_comercial</t>
         </is>
       </c>
     </row>
@@ -2938,7 +2938,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>36e9e6d</t>
+          <t>be2eeca</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
@@ -2948,12 +2948,12 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-10-22</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>Merge pull request #6 from aycaRichard12/develop</t>
+          <t>[񯢔] CAMBIO EN MAIN BAJARSE EN CADA REPOSITORIO : Se añadio el modal para registrar el punto de vent</t>
         </is>
       </c>
     </row>
@@ -2963,7 +2963,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>da93671</t>
+          <t>f6fb50b</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
@@ -2973,12 +2973,12 @@
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-10-21</t>
         </is>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>Merge pull request #5 from aycaRichard12/Feacture-Cotizacion_Detalle_Adicional_Cotizacion</t>
+          <t>[♦] se añadio trasabilidad en los movimientos de los productos esta en revision si funciona o hay conflicto con otras funciones</t>
         </is>
       </c>
     </row>
@@ -2988,7 +2988,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>0b50aa7</t>
+          <t>66c4346</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -2998,12 +2998,12 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>2025-10-18</t>
+          <t>2025-10-21</t>
         </is>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>[•] GOOD: se añadio descripcion adicional a cotizacion preferencial o normal en carrito para especificar los servicios tambien se añadio numero factura o ducumento a cotizaion tambien se muestra en los reportes dichos cambios</t>
+          <t>Merge pull request #9 from aycaRichard12/develop</t>
         </is>
       </c>
     </row>
@@ -3013,7 +3013,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>d5cf671</t>
+          <t>4dcd9af</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -3023,12 +3023,12 @@
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-21</t>
         </is>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>Merge pull request #4 from aycaRichard12/develop</t>
+          <t>[•] funciones para sacar reportes de los commits</t>
         </is>
       </c>
     </row>
@@ -3038,7 +3038,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>feb7ab7</t>
+          <t>45fd896</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
@@ -3048,12 +3048,12 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-20</t>
         </is>
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>Merge pull request #3 from aycaRichard12/Feacture-Detalle_Venta_Cotizacion</t>
+          <t>Merge pull request #8 from aycaRichard12/Feacture-punto_de_venta_cotizacion_facturacion</t>
         </is>
       </c>
     </row>
@@ -3063,7 +3063,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>0225d73</t>
+          <t>ff5c859</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -3073,12 +3073,12 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>2025-10-17</t>
+          <t>2025-10-20</t>
         </is>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>[•] Se agrego descripcion adicional en carrito fenta finalizado</t>
+          <t>[•] agregar marge adevelop</t>
         </is>
       </c>
     </row>
@@ -3088,7 +3088,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>89d2b1b</t>
+          <t>76114b3</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -3098,12 +3098,12 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-20</t>
         </is>
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>[•] Se añadio descripcion adicional en carrito ventas debajo de descripcion del producto</t>
+          <t>Merge pull request #7 from aycaRichard12/Feacture-punto_de_venta_cotizacion_facturacion</t>
         </is>
       </c>
     </row>
@@ -3113,7 +3113,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>2caed0c</t>
+          <t>5d0f3c8</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
@@ -3123,12 +3123,12 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-20</t>
         </is>
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>[◘] DEJAR DE RASTREAR .ENV EN DEVELOP</t>
+          <t>[•] Se añadio punto de venta a cotizaion y se muestra en los reportes tanto de venta y cotizacion</t>
         </is>
       </c>
     </row>
@@ -3138,7 +3138,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>21063fe</t>
+          <t>15d5fd2</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
@@ -3148,12 +3148,12 @@
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-20</t>
         </is>
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>[◘] DEJAR DE RASTREAR EL .ENV</t>
+          <t>[♦] PENDIENTE: SE AGREGO PUNTO DE VENTA A LOS REPORTES DE VENTAY SE REGISTRA EL PUNTO DE VENTA EN CADA COTIZACION Y SE ESTA VIENDO COLOCAR EL PUNTO DE VENTA EN LOS REPOSRTE Y FALTA REGISTRO DE ALMACEN</t>
         </is>
       </c>
     </row>
@@ -3163,7 +3163,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>3f1f7ca</t>
+          <t>36e9e6d</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
@@ -3173,12 +3173,12 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>Merge branch 'main' of https://github.com/aycaRichard12/Ms_comercial</t>
+          <t>Merge pull request #6 from aycaRichard12/develop</t>
         </is>
       </c>
     </row>
@@ -3188,7 +3188,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>a70e993</t>
+          <t>da93671</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
@@ -3198,12 +3198,12 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>[♦♦] CONFIG: gitignore</t>
+          <t>Merge pull request #5 from aycaRichard12/Feacture-Cotizacion_Detalle_Adicional_Cotizacion</t>
         </is>
       </c>
     </row>
@@ -3213,7 +3213,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>3b8119a</t>
+          <t>0b50aa7</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
@@ -3223,12 +3223,12 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-18</t>
         </is>
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>Merge pull request #2 from aycaRichard12/develop</t>
+          <t>[•] GOOD: se añadio descripcion adicional a cotizacion preferencial o normal en carrito para especificar los servicios tambien se añadio numero factura o ducumento a cotizaion tambien se muestra en los reportes dichos cambios</t>
         </is>
       </c>
     </row>
@@ -3238,7 +3238,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>ac09b1b</t>
+          <t>d5cf671</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
@@ -3248,12 +3248,12 @@
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>Merge branch 'main' into develop</t>
+          <t>Merge pull request #4 from aycaRichard12/develop</t>
         </is>
       </c>
     </row>
@@ -3263,7 +3263,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>8c87406</t>
+          <t>feb7ab7</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
@@ -3273,12 +3273,12 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>Merge pull request #1 from aycaRichard12/Feacture-kardex</t>
+          <t>Merge pull request #3 from aycaRichard12/Feacture-Detalle_Venta_Cotizacion</t>
         </is>
       </c>
     </row>
@@ -3288,7 +3288,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>40d7dc7</t>
+          <t>0225d73</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
@@ -3298,12 +3298,12 @@
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>2025-10-16</t>
+          <t>2025-10-17</t>
         </is>
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>Merge branch 'develop' of https://github.com/aycaRichard12/Ms_comercial into Feacture-kardex</t>
+          <t>[•] Se agrego descripcion adicional en carrito fenta finalizado</t>
         </is>
       </c>
     </row>
@@ -3313,7 +3313,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>8627407</t>
+          <t>89d2b1b</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
@@ -3323,12 +3323,12 @@
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>[•] Completado editar saldos eliminar y modal desplegable de los saldos de un producto seleccionado</t>
+          <t>[•] Se añadio descripcion adicional en carrito ventas debajo de descripcion del producto</t>
         </is>
       </c>
     </row>
@@ -3338,7 +3338,7 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>b1c23da</t>
+          <t>2caed0c</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
@@ -3348,12 +3348,12 @@
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>[♦] BUG MENU: se aumento en la funcion selectSubmenu otro else if para validar que si no tiene paginas el submenu entonces enrutar a la base del menu</t>
+          <t>[◘] DEJAR DE RASTREAR .ENV EN DEVELOP</t>
         </is>
       </c>
     </row>
@@ -3363,7 +3363,7 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>2578a08</t>
+          <t>21063fe</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
@@ -3373,12 +3373,12 @@
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>[•] BUG: correccion bug componente venta se mostraba a inicio sesion apezar de que no tenia permisos para mostrar</t>
+          <t>[◘] DEJAR DE RASTREAR EL .ENV</t>
         </is>
       </c>
     </row>
@@ -3388,7 +3388,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>92c2751</t>
+          <t>3f1f7ca</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
@@ -3398,12 +3398,12 @@
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>2025-10-15</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>[♦] BUG MENU: se aumento en la funcion selectSubmenu otro else if para validar que si no tiene paginas el submenu entonces enrutar a la base del menu</t>
+          <t>Merge branch 'main' of https://github.com/aycaRichard12/Ms_comercial</t>
         </is>
       </c>
     </row>
@@ -3413,7 +3413,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>af8a9eb</t>
+          <t>a70e993</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
@@ -3423,12 +3423,12 @@
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>[•] Iyeccion mistersoft esta fallando venta</t>
+          <t>[♦♦] CONFIG: gitignore</t>
         </is>
       </c>
     </row>
@@ -3438,7 +3438,7 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>bd7bea8</t>
+          <t>3b8119a</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
@@ -3448,12 +3448,12 @@
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>2025-10-14</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>[♦] Imcompleto cardex para mostrar detalle de saldo final</t>
+          <t>Merge pull request #2 from aycaRichard12/develop</t>
         </is>
       </c>
     </row>
@@ -3463,7 +3463,7 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>d331fac</t>
+          <t>ac09b1b</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
@@ -3473,12 +3473,12 @@
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>[♦] PENDIENTE KARDEX: se logro obtener el precio unitario de cada compra y su respectivo movimiento los negativos son salidas y los positivos son movimientos</t>
+          <t>Merge branch 'main' into develop</t>
         </is>
       </c>
     </row>
@@ -3488,7 +3488,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>0a097e1</t>
+          <t>8c87406</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
@@ -3498,12 +3498,12 @@
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>[•] BUG: correccion bug componente venta se mostraba a inicio sesion apezar de que no tenia permisos para mostrar</t>
+          <t>Merge pull request #1 from aycaRichard12/Feacture-kardex</t>
         </is>
       </c>
     </row>
@@ -3513,7 +3513,7 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>7a5032d</t>
+          <t>40d7dc7</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
@@ -3523,12 +3523,12 @@
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-16</t>
         </is>
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>[♦] IMCOMPLETO: NO SE TERMINO KARDEX</t>
+          <t>Merge branch 'develop' of https://github.com/aycaRichard12/Ms_comercial into Feacture-kardex</t>
         </is>
       </c>
     </row>
@@ -3538,7 +3538,7 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>85ed0f8</t>
+          <t>8627407</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
@@ -3548,12 +3548,12 @@
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>2025-10-11</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>[•] BUG: correccion bug componente venta se mostraba a inicio sesion apezar de que no tenia permisos para mostrar</t>
+          <t>[•] Completado editar saldos eliminar y modal desplegable de los saldos de un producto seleccionado</t>
         </is>
       </c>
     </row>
@@ -3563,7 +3563,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>1531505</t>
+          <t>b1c23da</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
@@ -3573,12 +3573,12 @@
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>2025-10-10</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>[•] BUG PERMISOS DE MENUS: se quito el direcionamiento automatico to:/ solo se opto por el @click</t>
+          <t>[♦] BUG MENU: se aumento en la funcion selectSubmenu otro else if para validar que si no tiene paginas el submenu entonces enrutar a la base del menu</t>
         </is>
       </c>
     </row>
@@ -3588,7 +3588,7 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>5b580ba</t>
+          <t>2578a08</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
@@ -3598,12 +3598,12 @@
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>2025-10-10</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>[•] COMPRA: modificar los btns reposrtes en select</t>
+          <t>[•] BUG: correccion bug componente venta se mostraba a inicio sesion apezar de que no tenia permisos para mostrar</t>
         </is>
       </c>
     </row>
@@ -3613,7 +3613,7 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>9f1a936</t>
+          <t>92c2751</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
@@ -3623,12 +3623,12 @@
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>2025-10-10</t>
+          <t>2025-10-15</t>
         </is>
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>[•] FINALIZACION FACTURA NOTA CREDITO: modificacion backen nota-credito - venta, modificacion front end combinar con contingencia</t>
+          <t>[♦] BUG MENU: se aumento en la funcion selectSubmenu otro else if para validar que si no tiene paginas el submenu entonces enrutar a la base del menu</t>
         </is>
       </c>
     </row>
@@ -3638,7 +3638,7 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>6faad43</t>
+          <t>af8a9eb</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
@@ -3648,12 +3648,12 @@
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>2025-10-07</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>[●] cambio tarjeta venta inicio a Resgistrar Venta</t>
+          <t>[•] Iyeccion mistersoft esta fallando venta</t>
         </is>
       </c>
     </row>
@@ -3663,7 +3663,7 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>bad185c</t>
+          <t>bd7bea8</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
@@ -3673,12 +3673,12 @@
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>2025-10-10</t>
+          <t>2025-10-14</t>
         </is>
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>[•] BUG PERMISOS DE MENUS: se quito el direcionamiento automatico to:/ solo se opto por el @click</t>
+          <t>[♦] Imcompleto cardex para mostrar detalle de saldo final</t>
         </is>
       </c>
     </row>
@@ -3688,7 +3688,7 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>e285b72</t>
+          <t>d331fac</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
@@ -3698,12 +3698,12 @@
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>2025-10-10</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>[•] BUG PERMISOS DE MENUS: se quito el direcionamiento automatico to:/ solo se opto por el @click</t>
+          <t>[♦] PENDIENTE KARDEX: se logro obtener el precio unitario de cada compra y su respectivo movimiento los negativos son salidas y los positivos son movimientos</t>
         </is>
       </c>
     </row>
@@ -3713,7 +3713,7 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>9aeafda</t>
+          <t>0a097e1</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
@@ -3723,12 +3723,12 @@
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>2025-10-10</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>[•] COMPRA: modificar los btns reposrtes en select</t>
+          <t>[•] BUG: correccion bug componente venta se mostraba a inicio sesion apezar de que no tenia permisos para mostrar</t>
         </is>
       </c>
     </row>
@@ -3738,7 +3738,7 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>7790afb</t>
+          <t>7a5032d</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
@@ -3748,12 +3748,12 @@
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>2025-10-10</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>[•] FINALIZACION FACTURA NOTA CREDITO: modificacion backen nota-credito - venta, modificacion front end combinar con contingencia</t>
+          <t>[♦] IMCOMPLETO: NO SE TERMINO KARDEX</t>
         </is>
       </c>
     </row>
@@ -3763,7 +3763,7 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>613a00f</t>
+          <t>85ed0f8</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
@@ -3773,12 +3773,12 @@
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>2025-10-09</t>
+          <t>2025-10-11</t>
         </is>
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>[NULL] PENDIENTE KARDEX : solo se quedo en obtner precios de las compras nos falta obtener UEPS PEPS Promedio</t>
+          <t>[•] BUG: correccion bug componente venta se mostraba a inicio sesion apezar de que no tenia permisos para mostrar</t>
         </is>
       </c>
     </row>
@@ -3788,7 +3788,7 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>4ce76ff</t>
+          <t>1531505</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
@@ -3798,12 +3798,12 @@
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>2025-10-07</t>
+          <t>2025-10-10</t>
         </is>
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>[●] cambio tarjeta venta inicio a Resgistrar Venta</t>
+          <t>[•] BUG PERMISOS DE MENUS: se quito el direcionamiento automatico to:/ solo se opto por el @click</t>
         </is>
       </c>
     </row>
@@ -3813,7 +3813,7 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>332f720</t>
+          <t>5b580ba</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
@@ -3823,12 +3823,12 @@
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>2025-10-07</t>
+          <t>2025-10-10</t>
         </is>
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>[■] MOD: Configuracion de TITLE PESTAÑA COMERCIAL y AUTOMATICO NOMBRE DE LA EMPRESA</t>
+          <t>[•] COMPRA: modificar los btns reposrtes en select</t>
         </is>
       </c>
     </row>
@@ -3838,7 +3838,7 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>28d88a6</t>
+          <t>9f1a936</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
@@ -3848,12 +3848,12 @@
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>2025-10-07</t>
+          <t>2025-10-10</t>
         </is>
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>[■] MOD : routes no mostrar rutas solo el link de version</t>
+          <t>[•] FINALIZACION FACTURA NOTA CREDITO: modificacion backen nota-credito - venta, modificacion front end combinar con contingencia</t>
         </is>
       </c>
     </row>
@@ -3863,7 +3863,7 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>d5a9711</t>
+          <t>6faad43</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
@@ -3878,7 +3878,7 @@
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>[■] MOD: Configuracion de TITLE PESTAÑA COMERCIAL y AUTOMATICO NOMBRE DE LA EMPRESA</t>
+          <t>[●] cambio tarjeta venta inicio a Resgistrar Venta</t>
         </is>
       </c>
     </row>
@@ -3888,7 +3888,7 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>7d8f950</t>
+          <t>bad185c</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
@@ -3898,12 +3898,12 @@
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>2025-10-07</t>
+          <t>2025-10-10</t>
         </is>
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>[●] MOD: actualizar tabla despues de registrar credito compra</t>
+          <t>[•] BUG PERMISOS DE MENUS: se quito el direcionamiento automatico to:/ solo se opto por el @click</t>
         </is>
       </c>
     </row>
@@ -3913,7 +3913,7 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>b51fb3d</t>
+          <t>e285b72</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
@@ -3923,12 +3923,12 @@
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>2025-10-07</t>
+          <t>2025-10-10</t>
         </is>
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>[●] MOD: no permite registrar dos veces para la misma compra</t>
+          <t>[•] BUG PERMISOS DE MENUS: se quito el direcionamiento automatico to:/ solo se opto por el @click</t>
         </is>
       </c>
     </row>
@@ -3938,7 +3938,7 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>d8a4322</t>
+          <t>9aeafda</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
@@ -3948,12 +3948,12 @@
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>2025-10-07</t>
+          <t>2025-10-10</t>
         </is>
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>[●] MOD: actualizar tabla despues de registrar credito compra</t>
+          <t>[•] COMPRA: modificar los btns reposrtes en select</t>
         </is>
       </c>
     </row>
@@ -3963,7 +3963,7 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>8262c38</t>
+          <t>7790afb</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
@@ -3973,12 +3973,12 @@
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t>2025-10-07</t>
+          <t>2025-10-10</t>
         </is>
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>[●] MOD: no permite registrar dos veces para la misma compra</t>
+          <t>[•] FINALIZACION FACTURA NOTA CREDITO: modificacion backen nota-credito - venta, modificacion front end combinar con contingencia</t>
         </is>
       </c>
     </row>
@@ -3988,7 +3988,7 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>cf100a2</t>
+          <t>613a00f</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
@@ -3998,12 +3998,12 @@
       </c>
       <c r="D143" t="inlineStr">
         <is>
-          <t>2025-10-07</t>
+          <t>2025-10-09</t>
         </is>
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>[◼︎] MOD: USUARIO DE PRUEBAS</t>
+          <t>[NULL] PENDIENTE KARDEX : solo se quedo en obtner precios de las compras nos falta obtener UEPS PEPS Promedio</t>
         </is>
       </c>
     </row>
@@ -4013,7 +4013,7 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>b5f2ef7</t>
+          <t>4ce76ff</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
@@ -4023,12 +4023,12 @@
       </c>
       <c r="D144" t="inlineStr">
         <is>
-          <t>2025-10-06</t>
+          <t>2025-10-07</t>
         </is>
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>MOD: arreglar routes</t>
+          <t>[●] cambio tarjeta venta inicio a Resgistrar Venta</t>
         </is>
       </c>
     </row>
@@ -4038,7 +4038,7 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>3be4789</t>
+          <t>332f720</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
@@ -4048,12 +4048,12 @@
       </c>
       <c r="D145" t="inlineStr">
         <is>
-          <t>2025-10-06</t>
+          <t>2025-10-07</t>
         </is>
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t>[☺] MOD: REPORTE MERMA Y EXTRAVIO Y SELECT REPORTE</t>
+          <t>[■] MOD: Configuracion de TITLE PESTAÑA COMERCIAL y AUTOMATICO NOMBRE DE LA EMPRESA</t>
         </is>
       </c>
     </row>
@@ -4063,7 +4063,7 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>5a87c4c</t>
+          <t>28d88a6</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
@@ -4073,12 +4073,12 @@
       </c>
       <c r="D146" t="inlineStr">
         <is>
-          <t>2025-10-06</t>
+          <t>2025-10-07</t>
         </is>
       </c>
       <c r="E146" t="inlineStr">
         <is>
-          <t>MOD: arreglar routes</t>
+          <t>[■] MOD : routes no mostrar rutas solo el link de version</t>
         </is>
       </c>
     </row>
@@ -4088,7 +4088,7 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>fef5258</t>
+          <t>d5a9711</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
@@ -4098,12 +4098,12 @@
       </c>
       <c r="D147" t="inlineStr">
         <is>
-          <t>2025-10-06</t>
+          <t>2025-10-07</t>
         </is>
       </c>
       <c r="E147" t="inlineStr">
         <is>
-          <t>[☺] MOD: REPORTE MERMA Y EXTRAVIO Y SELECT REPORTE</t>
+          <t>[■] MOD: Configuracion de TITLE PESTAÑA COMERCIAL y AUTOMATICO NOMBRE DE LA EMPRESA</t>
         </is>
       </c>
     </row>
@@ -4113,7 +4113,7 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>fd450ca</t>
+          <t>7d8f950</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
@@ -4123,12 +4123,12 @@
       </c>
       <c r="D148" t="inlineStr">
         <is>
-          <t>2025-10-04</t>
+          <t>2025-10-07</t>
         </is>
       </c>
       <c r="E148" t="inlineStr">
         <is>
-          <t>eliminar de routes inventarios kardexPage</t>
+          <t>[●] MOD: actualizar tabla despues de registrar credito compra</t>
         </is>
       </c>
     </row>
@@ -4138,7 +4138,7 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>991ae7c</t>
+          <t>b51fb3d</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
@@ -4148,12 +4148,12 @@
       </c>
       <c r="D149" t="inlineStr">
         <is>
-          <t>2025-10-04</t>
+          <t>2025-10-07</t>
         </is>
       </c>
       <c r="E149" t="inlineStr">
         <is>
-          <t>eliminar de routes inventarios kardexPage</t>
+          <t>[●] MOD: no permite registrar dos veces para la misma compra</t>
         </is>
       </c>
     </row>
@@ -4163,7 +4163,7 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>67469e9</t>
+          <t>d8a4322</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
@@ -4173,12 +4173,12 @@
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>2025-10-04</t>
+          <t>2025-10-07</t>
         </is>
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t>[☺] Mod : cerrar modal (registrar usuario responsable) despues de registrar - cambiar label btn de guardar por aprobado</t>
+          <t>[●] MOD: actualizar tabla despues de registrar credito compra</t>
         </is>
       </c>
     </row>
@@ -4188,7 +4188,7 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>4afec30</t>
+          <t>8262c38</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
@@ -4198,12 +4198,12 @@
       </c>
       <c r="D151" t="inlineStr">
         <is>
-          <t>2025-10-04</t>
+          <t>2025-10-07</t>
         </is>
       </c>
       <c r="E151" t="inlineStr">
         <is>
-          <t>[■] MOD .env para develop</t>
+          <t>[●] MOD: no permite registrar dos veces para la misma compra</t>
         </is>
       </c>
     </row>
@@ -4213,7 +4213,7 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>a5e2ba8</t>
+          <t>cf100a2</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
@@ -4223,12 +4223,12 @@
       </c>
       <c r="D152" t="inlineStr">
         <is>
-          <t>2025-10-04</t>
+          <t>2025-10-07</t>
         </is>
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>[☺] Mod : cerrar modal (registrar usuario responsable) despues de registrar - cambiar label btn de guardar por aprobado</t>
+          <t>[◼︎] MOD: USUARIO DE PRUEBAS</t>
         </is>
       </c>
     </row>
@@ -4238,7 +4238,7 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>51f047d</t>
+          <t>b5f2ef7</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
@@ -4248,12 +4248,12 @@
       </c>
       <c r="D153" t="inlineStr">
         <is>
-          <t>2025-10-04</t>
+          <t>2025-10-06</t>
         </is>
       </c>
       <c r="E153" t="inlineStr">
         <is>
-          <t>[○] -&gt; Mod Filtrado precio sugerido, Filtrado costo unitaro DC : fitrar a inicio</t>
+          <t>MOD: arreglar routes</t>
         </is>
       </c>
     </row>
@@ -4263,7 +4263,7 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>bef63cc</t>
+          <t>3be4789</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
@@ -4273,12 +4273,12 @@
       </c>
       <c r="D154" t="inlineStr">
         <is>
-          <t>2025-10-04</t>
+          <t>2025-10-06</t>
         </is>
       </c>
       <c r="E154" t="inlineStr">
         <is>
-          <t>[○] -&gt; Mod Filtrado precio sugerido, Filtrado costo unitaro DC : fitrar a inicio</t>
+          <t>[☺] MOD: REPORTE MERMA Y EXTRAVIO Y SELECT REPORTE</t>
         </is>
       </c>
     </row>
@@ -4288,7 +4288,7 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>0d3e4c2</t>
+          <t>5a87c4c</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
@@ -4298,12 +4298,12 @@
       </c>
       <c r="D155" t="inlineStr">
         <is>
-          <t>2025-10-04</t>
+          <t>2025-10-06</t>
         </is>
       </c>
       <c r="E155" t="inlineStr">
         <is>
-          <t>[■] configuracion develop terminada - estructura usuarios de pruebas - quasar config</t>
+          <t>MOD: arreglar routes</t>
         </is>
       </c>
     </row>
@@ -4313,7 +4313,7 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>b14e001</t>
+          <t>fef5258</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
@@ -4323,12 +4323,12 @@
       </c>
       <c r="D156" t="inlineStr">
         <is>
-          <t>2025-10-03</t>
+          <t>2025-10-06</t>
         </is>
       </c>
       <c r="E156" t="inlineStr">
         <is>
-          <t>cambio axios + .nev para produccion, mod services con .env, mod usuarios para pruebas locales y produccion, mod credeciales usuarios para inicialisar en desarrollo no afecta a produccion</t>
+          <t>[☺] MOD: REPORTE MERMA Y EXTRAVIO Y SELECT REPORTE</t>
         </is>
       </c>
     </row>
@@ -4338,7 +4338,7 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>99c04fd</t>
+          <t>fd450ca</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
@@ -4348,12 +4348,12 @@
       </c>
       <c r="D157" t="inlineStr">
         <is>
-          <t>2025-10-03</t>
+          <t>2025-10-04</t>
         </is>
       </c>
       <c r="E157" t="inlineStr">
         <is>
-          <t>cambios .env si se subira al git no se ignorara</t>
+          <t>eliminar de routes inventarios kardexPage</t>
         </is>
       </c>
     </row>
@@ -4363,7 +4363,7 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>91897d7</t>
+          <t>991ae7c</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
@@ -4373,12 +4373,12 @@
       </c>
       <c r="D158" t="inlineStr">
         <is>
-          <t>2025-10-03</t>
+          <t>2025-10-04</t>
         </is>
       </c>
       <c r="E158" t="inlineStr">
         <is>
-          <t>configuraicion develop .env, configuracion axios api, confg de services apis externas -&gt; servidor de prueva para hacer lo minimos cambios</t>
+          <t>eliminar de routes inventarios kardexPage</t>
         </is>
       </c>
     </row>
@@ -4388,7 +4388,7 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>67b9aa5</t>
+          <t>67469e9</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
@@ -4398,12 +4398,12 @@
       </c>
       <c r="D159" t="inlineStr">
         <is>
-          <t>2025-10-03</t>
+          <t>2025-10-04</t>
         </is>
       </c>
       <c r="E159" t="inlineStr">
         <is>
-          <t>hacer cambios reporte cuentas por cobrar al generar reporte scroll se posiciona en tabla, añadir kardex a select reportes comiezo de git con ramas</t>
+          <t>[☺] Mod : cerrar modal (registrar usuario responsable) despues de registrar - cambiar label btn de guardar por aprobado</t>
         </is>
       </c>
     </row>
@@ -4413,7 +4413,7 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>62dbbab</t>
+          <t>4afec30</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
@@ -4423,12 +4423,12 @@
       </c>
       <c r="D160" t="inlineStr">
         <is>
-          <t>2025-10-02</t>
+          <t>2025-10-04</t>
         </is>
       </c>
       <c r="E160" t="inlineStr">
         <is>
-          <t>correcciones comercial</t>
+          <t>[■] MOD .env para develop</t>
         </is>
       </c>
     </row>
@@ -4438,7 +4438,7 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>3e0caaa</t>
+          <t>a5e2ba8</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
@@ -4448,12 +4448,12 @@
       </c>
       <c r="D161" t="inlineStr">
         <is>
-          <t>2025-09-19</t>
+          <t>2025-10-04</t>
         </is>
       </c>
       <c r="E161" t="inlineStr">
         <is>
-          <t>cambios comercial -NO SE TERMINO COMERCIAL- -se hizo cambios menus falta terminar reportes-</t>
+          <t>[☺] Mod : cerrar modal (registrar usuario responsable) despues de registrar - cambiar label btn de guardar por aprobado</t>
         </is>
       </c>
     </row>
@@ -4463,7 +4463,7 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>3a1565d</t>
+          <t>51f047d</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
@@ -4473,12 +4473,12 @@
       </c>
       <c r="D162" t="inlineStr">
         <is>
-          <t>2025-09-16</t>
+          <t>2025-10-04</t>
         </is>
       </c>
       <c r="E162" t="inlineStr">
         <is>
-          <t>desarrollo ota deito credito</t>
+          <t>[○] -&gt; Mod Filtrado precio sugerido, Filtrado costo unitaro DC : fitrar a inicio</t>
         </is>
       </c>
     </row>
@@ -4488,7 +4488,7 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>412b529</t>
+          <t>bef63cc</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
@@ -4498,12 +4498,12 @@
       </c>
       <c r="D163" t="inlineStr">
         <is>
-          <t>2025-09-11</t>
+          <t>2025-10-04</t>
         </is>
       </c>
       <c r="E163" t="inlineStr">
         <is>
-          <t>Commmit : Solucion de Error Devolucion Venta / mejora de reportes de Venta Gris</t>
+          <t>[○] -&gt; Mod Filtrado precio sugerido, Filtrado costo unitaro DC : fitrar a inicio</t>
         </is>
       </c>
     </row>
@@ -4513,7 +4513,7 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>7cd7d32</t>
+          <t>0d3e4c2</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
@@ -4523,12 +4523,12 @@
       </c>
       <c r="D164" t="inlineStr">
         <is>
-          <t>2025-09-10</t>
+          <t>2025-10-04</t>
         </is>
       </c>
       <c r="E164" t="inlineStr">
         <is>
-          <t>Api Compra Out y Diseño Estructura Guias Interfaz Quasar y Dirver</t>
+          <t>[■] configuracion develop terminada - estructura usuarios de pruebas - quasar config</t>
         </is>
       </c>
     </row>
@@ -4538,7 +4538,7 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>a449083</t>
+          <t>b14e001</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
@@ -4548,12 +4548,12 @@
       </c>
       <c r="D165" t="inlineStr">
         <is>
-          <t>2025-09-09</t>
+          <t>2025-10-03</t>
         </is>
       </c>
       <c r="E165" t="inlineStr">
         <is>
-          <t>Api out ventas finalzida con los parametros optimizados</t>
+          <t>cambio axios + .nev para produccion, mod services con .env, mod usuarios para pruebas locales y produccion, mod credeciales usuarios para inicialisar en desarrollo no afecta a produccion</t>
         </is>
       </c>
     </row>
@@ -4563,7 +4563,7 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>b451274</t>
+          <t>99c04fd</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
@@ -4573,12 +4573,12 @@
       </c>
       <c r="D166" t="inlineStr">
         <is>
-          <t>2025-09-03</t>
+          <t>2025-10-03</t>
         </is>
       </c>
       <c r="E166" t="inlineStr">
         <is>
-          <t>compra creditos</t>
+          <t>cambios .env si se subira al git no se ignorara</t>
         </is>
       </c>
     </row>
@@ -4588,7 +4588,7 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>dd40fa0</t>
+          <t>91897d7</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
@@ -4598,12 +4598,12 @@
       </c>
       <c r="D167" t="inlineStr">
         <is>
-          <t>2025-09-02</t>
+          <t>2025-10-03</t>
         </is>
       </c>
       <c r="E167" t="inlineStr">
         <is>
-          <t>m:correcciones comercial</t>
+          <t>configuraicion develop .env, configuracion axios api, confg de services apis externas -&gt; servidor de prueva para hacer lo minimos cambios</t>
         </is>
       </c>
     </row>
@@ -4613,7 +4613,7 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>da37a18</t>
+          <t>67b9aa5</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
@@ -4623,12 +4623,12 @@
       </c>
       <c r="D168" t="inlineStr">
         <is>
-          <t>2025-08-30</t>
+          <t>2025-10-03</t>
         </is>
       </c>
       <c r="E168" t="inlineStr">
         <is>
-          <t>Cambios Sistema correcciones primera interacion</t>
+          <t>hacer cambios reporte cuentas por cobrar al generar reporte scroll se posiciona en tabla, añadir kardex a select reportes comiezo de git con ramas</t>
         </is>
       </c>
     </row>
@@ -4638,7 +4638,7 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>f5c4d75</t>
+          <t>62dbbab</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
@@ -4648,12 +4648,12 @@
       </c>
       <c r="D169" t="inlineStr">
         <is>
-          <t>2025-08-01</t>
+          <t>2025-10-02</t>
         </is>
       </c>
       <c r="E169" t="inlineStr">
         <is>
-          <t>Cambios interfaz</t>
+          <t>correcciones comercial</t>
         </is>
       </c>
     </row>
@@ -4663,7 +4663,7 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>283842d</t>
+          <t>3e0caaa</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
@@ -4673,12 +4673,12 @@
       </c>
       <c r="D170" t="inlineStr">
         <is>
-          <t>2025-06-19</t>
+          <t>2025-09-19</t>
         </is>
       </c>
       <c r="E170" t="inlineStr">
         <is>
-          <t>Eliminar vendor del repo y agregarlo al .gitignore</t>
+          <t>cambios comercial -NO SE TERMINO COMERCIAL- -se hizo cambios menus falta terminar reportes-</t>
         </is>
       </c>
     </row>
@@ -4688,7 +4688,7 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>3501c4e</t>
+          <t>3a1565d</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
@@ -4698,12 +4698,12 @@
       </c>
       <c r="D171" t="inlineStr">
         <is>
-          <t>2025-04-21</t>
+          <t>2025-09-16</t>
         </is>
       </c>
       <c r="E171" t="inlineStr">
         <is>
-          <t>first commit</t>
+          <t>desarrollo ota deito credito</t>
         </is>
       </c>
     </row>
@@ -4713,20 +4713,245 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
+          <t>412b529</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>aycaRichard12</t>
+        </is>
+      </c>
+      <c r="D172" t="inlineStr">
+        <is>
+          <t>2025-09-11</t>
+        </is>
+      </c>
+      <c r="E172" t="inlineStr">
+        <is>
+          <t>Commmit : Solucion de Error Devolucion Venta / mejora de reportes de Venta Gris</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="n">
+        <v>171</v>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>7cd7d32</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>aycaRichard12</t>
+        </is>
+      </c>
+      <c r="D173" t="inlineStr">
+        <is>
+          <t>2025-09-10</t>
+        </is>
+      </c>
+      <c r="E173" t="inlineStr">
+        <is>
+          <t>Api Compra Out y Diseño Estructura Guias Interfaz Quasar y Dirver</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="n">
+        <v>172</v>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>a449083</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>aycaRichard12</t>
+        </is>
+      </c>
+      <c r="D174" t="inlineStr">
+        <is>
+          <t>2025-09-09</t>
+        </is>
+      </c>
+      <c r="E174" t="inlineStr">
+        <is>
+          <t>Api out ventas finalzida con los parametros optimizados</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="n">
+        <v>173</v>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>b451274</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>aycaRichard12</t>
+        </is>
+      </c>
+      <c r="D175" t="inlineStr">
+        <is>
+          <t>2025-09-03</t>
+        </is>
+      </c>
+      <c r="E175" t="inlineStr">
+        <is>
+          <t>compra creditos</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="n">
+        <v>174</v>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>dd40fa0</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>aycaRichard12</t>
+        </is>
+      </c>
+      <c r="D176" t="inlineStr">
+        <is>
+          <t>2025-09-02</t>
+        </is>
+      </c>
+      <c r="E176" t="inlineStr">
+        <is>
+          <t>m:correcciones comercial</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="n">
+        <v>175</v>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>da37a18</t>
+        </is>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>aycaRichard12</t>
+        </is>
+      </c>
+      <c r="D177" t="inlineStr">
+        <is>
+          <t>2025-08-30</t>
+        </is>
+      </c>
+      <c r="E177" t="inlineStr">
+        <is>
+          <t>Cambios Sistema correcciones primera interacion</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="n">
+        <v>176</v>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>f5c4d75</t>
+        </is>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>aycaRichard12</t>
+        </is>
+      </c>
+      <c r="D178" t="inlineStr">
+        <is>
+          <t>2025-08-01</t>
+        </is>
+      </c>
+      <c r="E178" t="inlineStr">
+        <is>
+          <t>Cambios interfaz</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="n">
+        <v>177</v>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>283842d</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>aycaRichard12</t>
+        </is>
+      </c>
+      <c r="D179" t="inlineStr">
+        <is>
+          <t>2025-06-19</t>
+        </is>
+      </c>
+      <c r="E179" t="inlineStr">
+        <is>
+          <t>Eliminar vendor del repo y agregarlo al .gitignore</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="n">
+        <v>178</v>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>3501c4e</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>aycaRichard12</t>
+        </is>
+      </c>
+      <c r="D180" t="inlineStr">
+        <is>
+          <t>2025-04-21</t>
+        </is>
+      </c>
+      <c r="E180" t="inlineStr">
+        <is>
+          <t>first commit</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="n">
+        <v>179</v>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
           <t>9409db8</t>
         </is>
       </c>
-      <c r="C172" t="inlineStr">
+      <c r="C181" t="inlineStr">
         <is>
           <t>Ricahrd Ayca</t>
         </is>
       </c>
-      <c r="D172" t="inlineStr">
+      <c r="D181" t="inlineStr">
         <is>
           <t>2025-04-01</t>
         </is>
       </c>
-      <c r="E172" t="inlineStr">
+      <c r="E181" t="inlineStr">
         <is>
           <t>Initialize the project 🚀</t>
         </is>

</xml_diff>